<commit_message>
fixed model lambda setting
</commit_message>
<xml_diff>
--- a/outcome/appendix/Figure Data/Fig.3 data.xlsx
+++ b/outcome/appendix/Figure Data/Fig.3 data.xlsx
@@ -488,16 +488,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.14</v>
+        <v>0.14</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.26</v>
+        <v>0.26</v>
       </c>
       <c r="F2" t="n">
-        <v>0.22</v>
+        <v>-0.22</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.11</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3">
@@ -511,16 +511,16 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.21</v>
+        <v>0.21</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09</v>
+        <v>-0.09</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.22</v>
+        <v>0.22</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.08</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4">
@@ -534,16 +534,16 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.89</v>
+        <v>0.89</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.57</v>
+        <v>0.57</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.21</v>
+        <v>0.21</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
@@ -557,16 +557,16 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.61</v>
+        <v>2.61</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.79</v>
+        <v>0.79</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.09</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="6">
@@ -580,16 +580,16 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.86</v>
+        <v>1.86</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.49</v>
+        <v>0.49</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.86</v>
+        <v>0.86</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7">
@@ -603,16 +603,16 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>5.7</v>
+        <v>-5.7</v>
       </c>
       <c r="E7" t="n">
-        <v>1.96</v>
+        <v>-1.96</v>
       </c>
       <c r="F7" t="n">
-        <v>1.87</v>
+        <v>-1.87</v>
       </c>
       <c r="G7" t="n">
-        <v>1.88</v>
+        <v>-1.88</v>
       </c>
     </row>
     <row r="8">
@@ -626,16 +626,16 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.66</v>
+        <v>0.66</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.11</v>
+        <v>0.11</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.21</v>
+        <v>0.21</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.34</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="9">
@@ -649,16 +649,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.42</v>
+        <v>1.42</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.54</v>
+        <v>0.54</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.43</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="10">
@@ -672,16 +672,16 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1.97</v>
+        <v>-1.97</v>
       </c>
       <c r="E10" t="n">
-        <v>0.71</v>
+        <v>-0.71</v>
       </c>
       <c r="F10" t="n">
-        <v>0.58</v>
+        <v>-0.58</v>
       </c>
       <c r="G10" t="n">
-        <v>0.69</v>
+        <v>-0.69</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.79</v>
+        <v>2.79</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.96</v>
+        <v>0.96</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.91</v>
+        <v>0.91</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.91</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="12">
@@ -718,16 +718,16 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.19</v>
+        <v>2.19</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.74</v>
+        <v>0.74</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.74</v>
+        <v>0.74</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.71</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="13">
@@ -741,16 +741,16 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>5.09</v>
+        <v>-5.09</v>
       </c>
       <c r="E13" t="n">
-        <v>1.65</v>
+        <v>-1.65</v>
       </c>
       <c r="F13" t="n">
-        <v>1.74</v>
+        <v>-1.74</v>
       </c>
       <c r="G13" t="n">
-        <v>1.7</v>
+        <v>-1.7</v>
       </c>
     </row>
     <row r="14">
@@ -764,16 +764,16 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.49</v>
+        <v>1.49</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.46</v>
+        <v>0.46</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.43</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="15">
@@ -787,16 +787,16 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.87</v>
+        <v>-0.87</v>
       </c>
       <c r="E15" t="n">
-        <v>1.15</v>
+        <v>-1.15</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.12</v>
+        <v>0.12</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.16</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="16">
@@ -810,16 +810,16 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.81</v>
+        <v>1.81</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.74</v>
+        <v>0.74</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.52</v>
+        <v>0.52</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.55</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="17">
@@ -833,16 +833,16 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.63</v>
+        <v>1.63</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.66</v>
+        <v>0.66</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.49</v>
+        <v>0.49</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.48</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="18">
@@ -856,16 +856,16 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.4</v>
+        <v>1.4</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.58</v>
+        <v>0.58</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.41</v>
+        <v>0.41</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.41</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="19">
@@ -879,16 +879,16 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>5.46</v>
+        <v>-5.46</v>
       </c>
       <c r="E19" t="n">
-        <v>1.41</v>
+        <v>-1.41</v>
       </c>
       <c r="F19" t="n">
-        <v>2.02</v>
+        <v>-2.02</v>
       </c>
       <c r="G19" t="n">
-        <v>2.02</v>
+        <v>-2.02</v>
       </c>
     </row>
     <row r="20">
@@ -902,16 +902,16 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.13</v>
+        <v>0.13</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.84</v>
+        <v>0.84</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.07</v>
+        <v>1.07</v>
       </c>
       <c r="G20" t="n">
-        <v>1.79</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="21">
@@ -925,16 +925,16 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1.71</v>
+        <v>-1.71</v>
       </c>
       <c r="E21" t="n">
-        <v>1.43</v>
+        <v>-1.43</v>
       </c>
       <c r="F21" t="n">
-        <v>0.76</v>
+        <v>-0.76</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.47</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="22">
@@ -948,16 +948,16 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.67</v>
+        <v>1.67</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.63</v>
+        <v>0.63</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.56</v>
+        <v>0.56</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.48</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="23">
@@ -971,16 +971,16 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-1.6</v>
+        <v>1.6</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
       <c r="F23" t="n">
-        <v>-1.05</v>
+        <v>1.05</v>
       </c>
       <c r="G23" t="n">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="24">
@@ -994,16 +994,16 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.22</v>
+        <v>0.22</v>
       </c>
       <c r="F24" t="n">
-        <v>0.93</v>
+        <v>-0.93</v>
       </c>
       <c r="G24" t="n">
-        <v>0.04</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="25">
@@ -1017,16 +1017,16 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.94</v>
+        <v>-0.94</v>
       </c>
       <c r="E25" t="n">
-        <v>1.08</v>
+        <v>-1.08</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.13</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="26">
@@ -1040,16 +1040,16 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>5.22</v>
+        <v>-5.22</v>
       </c>
       <c r="E26" t="n">
-        <v>1.92</v>
+        <v>-1.92</v>
       </c>
       <c r="F26" t="n">
-        <v>1.34</v>
+        <v>-1.34</v>
       </c>
       <c r="G26" t="n">
-        <v>1.97</v>
+        <v>-1.97</v>
       </c>
     </row>
     <row r="27">
@@ -1063,16 +1063,16 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-1.83</v>
+        <v>1.83</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.53</v>
+        <v>0.53</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.59</v>
+        <v>0.59</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="28">
@@ -1086,16 +1086,16 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.38</v>
+        <v>0.38</v>
       </c>
       <c r="F28" t="n">
-        <v>0.06</v>
+        <v>-0.06</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.69</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="29">
@@ -1109,16 +1109,16 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.48</v>
+        <v>0.48</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.18</v>
+        <v>0.18</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.27</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="30">
@@ -1132,16 +1132,16 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>-2.72</v>
+        <v>2.72</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.92</v>
+        <v>0.92</v>
       </c>
       <c r="F30" t="n">
-        <v>-1.52</v>
+        <v>1.52</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.28</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="31">
@@ -1155,16 +1155,16 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.81</v>
+        <v>-0.81</v>
       </c>
       <c r="E31" t="n">
-        <v>0.09</v>
+        <v>-0.09</v>
       </c>
       <c r="F31" t="n">
-        <v>0.74</v>
+        <v>-0.74</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="32">
@@ -1178,16 +1178,16 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.19</v>
+        <v>-0.19</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
       <c r="F32" t="n">
-        <v>-1.05</v>
+        <v>1.05</v>
       </c>
       <c r="G32" t="n">
-        <v>1.94</v>
+        <v>-1.94</v>
       </c>
     </row>
     <row r="33">
@@ -1201,16 +1201,16 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>-1.73</v>
+        <v>1.73</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.24</v>
+        <v>0.24</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.74</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="34">
@@ -1224,16 +1224,16 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>-1.06</v>
+        <v>1.06</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.67</v>
+        <v>0.67</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.28</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="35">
@@ -1247,16 +1247,16 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>2.09</v>
+        <v>-2.09</v>
       </c>
       <c r="E35" t="n">
-        <v>0.85</v>
+        <v>-0.85</v>
       </c>
       <c r="F35" t="n">
-        <v>1.1</v>
+        <v>-1.1</v>
       </c>
       <c r="G35" t="n">
-        <v>0.14</v>
+        <v>-0.14</v>
       </c>
     </row>
     <row r="36">
@@ -1270,16 +1270,16 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.77</v>
+        <v>0.77</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.42</v>
+        <v>0.42</v>
       </c>
       <c r="F36" t="n">
-        <v>0.07</v>
+        <v>-0.07</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.42</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="37">
@@ -1293,16 +1293,16 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>2.21</v>
+        <v>-2.21</v>
       </c>
       <c r="E37" t="n">
-        <v>1.56</v>
+        <v>-1.56</v>
       </c>
       <c r="F37" t="n">
-        <v>1.29</v>
+        <v>-1.29</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.64</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="38">
@@ -1316,16 +1316,16 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>-1.85</v>
+        <v>1.85</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.57</v>
+        <v>0.57</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.56</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="39">
@@ -1339,16 +1339,16 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
+        <v>-1.15</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.79</v>
+      </c>
+      <c r="G39" t="n">
         <v>1.15</v>
-      </c>
-      <c r="E39" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="G39" t="n">
-        <v>-1.15</v>
       </c>
     </row>
     <row r="40">
@@ -1362,16 +1362,16 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.79</v>
+        <v>-0.79</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.44</v>
+        <v>0.44</v>
       </c>
       <c r="G40" t="n">
-        <v>1.62</v>
+        <v>-1.62</v>
       </c>
     </row>
     <row r="41">
@@ -1385,16 +1385,16 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>-1.3</v>
+        <v>1.3</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.97</v>
+        <v>0.97</v>
       </c>
       <c r="G41" t="n">
-        <v>0.39</v>
+        <v>-0.39</v>
       </c>
     </row>
     <row r="42">
@@ -1408,16 +1408,16 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>-1.83</v>
+        <v>1.83</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.46</v>
+        <v>0.46</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.67</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="43">
@@ -1431,16 +1431,16 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>3.04</v>
+        <v>-3.04</v>
       </c>
       <c r="E43" t="n">
-        <v>1.04</v>
+        <v>-1.04</v>
       </c>
       <c r="F43" t="n">
-        <v>1.64</v>
+        <v>-1.64</v>
       </c>
       <c r="G43" t="n">
-        <v>0.36</v>
+        <v>-0.36</v>
       </c>
     </row>
     <row r="44">
@@ -1454,16 +1454,16 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>5.11</v>
+        <v>-5.11</v>
       </c>
       <c r="E44" t="n">
-        <v>1.84</v>
+        <v>-1.84</v>
       </c>
       <c r="F44" t="n">
-        <v>1.75</v>
+        <v>-1.75</v>
       </c>
       <c r="G44" t="n">
-        <v>1.52</v>
+        <v>-1.52</v>
       </c>
     </row>
     <row r="45">
@@ -1477,16 +1477,16 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>-1.25</v>
+        <v>1.25</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="46">
@@ -1500,16 +1500,16 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>-1.83</v>
+        <v>1.83</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.59</v>
+        <v>0.59</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.56</v>
+        <v>0.56</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="47">
@@ -1523,13 +1523,13 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.84</v>
+        <v>-0.84</v>
       </c>
       <c r="E47" t="n">
-        <v>0.36</v>
+        <v>-0.36</v>
       </c>
       <c r="F47" t="n">
-        <v>0.49</v>
+        <v>-0.49</v>
       </c>
       <c r="G47"/>
     </row>
@@ -1544,16 +1544,16 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.07</v>
+        <v>-0.07</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.22</v>
+        <v>0.22</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.18</v>
+        <v>0.18</v>
       </c>
       <c r="G48" t="n">
-        <v>0.47</v>
+        <v>-0.47</v>
       </c>
     </row>
     <row r="49">
@@ -1567,16 +1567,16 @@
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>-2.95</v>
+        <v>2.95</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.94</v>
+        <v>0.94</v>
       </c>
       <c r="F49" t="n">
-        <v>-1.1</v>
+        <v>1.1</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.91</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="50">
@@ -1590,16 +1590,16 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>4.1</v>
+        <v>-4.1</v>
       </c>
       <c r="E50" t="n">
-        <v>1.41</v>
+        <v>-1.41</v>
       </c>
       <c r="F50" t="n">
-        <v>1.45</v>
+        <v>-1.45</v>
       </c>
       <c r="G50" t="n">
-        <v>1.24</v>
+        <v>-1.24</v>
       </c>
     </row>
     <row r="51">
@@ -1613,16 +1613,16 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>3.54</v>
+        <v>-3.54</v>
       </c>
       <c r="E51" t="n">
-        <v>1.15</v>
+        <v>-1.15</v>
       </c>
       <c r="F51" t="n">
-        <v>1.1</v>
+        <v>-1.1</v>
       </c>
       <c r="G51" t="n">
-        <v>1.3</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="52">
@@ -1636,16 +1636,16 @@
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>-1.71</v>
+        <v>1.71</v>
       </c>
       <c r="E52" t="n">
-        <v>-0.58</v>
+        <v>0.58</v>
       </c>
       <c r="F52" t="n">
-        <v>-0.53</v>
+        <v>0.53</v>
       </c>
       <c r="G52" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="53">
@@ -1659,16 +1659,16 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>-1.94</v>
+        <v>1.94</v>
       </c>
       <c r="E53" t="n">
-        <v>-0.48</v>
+        <v>0.48</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.49</v>
+        <v>0.49</v>
       </c>
       <c r="G53" t="n">
-        <v>-0.97</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="54">
@@ -1682,16 +1682,16 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>-1.81</v>
+        <v>1.81</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.69</v>
+        <v>0.69</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
       <c r="G54" t="n">
-        <v>-0.42</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="55">
@@ -1705,16 +1705,16 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>-2.18</v>
+        <v>2.18</v>
       </c>
       <c r="E55" t="n">
-        <v>-0.81</v>
+        <v>0.81</v>
       </c>
       <c r="F55" t="n">
-        <v>-0.82</v>
+        <v>0.82</v>
       </c>
       <c r="G55" t="n">
-        <v>-0.55</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="56">
@@ -1728,16 +1728,16 @@
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>4.18</v>
+        <v>-4.18</v>
       </c>
       <c r="E56" t="n">
-        <v>1.63</v>
+        <v>-1.63</v>
       </c>
       <c r="F56" t="n">
-        <v>1.8</v>
+        <v>-1.8</v>
       </c>
       <c r="G56" t="n">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="57">
@@ -1751,16 +1751,16 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>1.33</v>
+        <v>-1.33</v>
       </c>
       <c r="E57" t="n">
-        <v>0.23</v>
+        <v>-0.23</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="G57" t="n">
-        <v>1.13</v>
+        <v>-1.13</v>
       </c>
     </row>
     <row r="58">
@@ -1774,16 +1774,16 @@
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.63</v>
+        <v>-0.63</v>
       </c>
       <c r="E58" t="n">
-        <v>0.53</v>
+        <v>-0.53</v>
       </c>
       <c r="F58" t="n">
-        <v>0.29</v>
+        <v>-0.29</v>
       </c>
       <c r="G58" t="n">
-        <v>-0.19</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="59">
@@ -1797,16 +1797,16 @@
         <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>-3.87</v>
+        <v>3.87</v>
       </c>
       <c r="E59" t="n">
-        <v>-1.02</v>
+        <v>1.02</v>
       </c>
       <c r="F59" t="n">
-        <v>-1.1</v>
+        <v>1.1</v>
       </c>
       <c r="G59" t="n">
-        <v>-1.74</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="60">
@@ -1820,16 +1820,16 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.78</v>
+        <v>0.78</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.65</v>
+        <v>0.65</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.35</v>
+        <v>0.35</v>
       </c>
       <c r="G60" t="n">
-        <v>0.21</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="61">
@@ -1843,16 +1843,16 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="E61" t="n">
-        <v>-0.73</v>
+        <v>0.73</v>
       </c>
       <c r="F61" t="n">
-        <v>-0.61</v>
+        <v>0.61</v>
       </c>
       <c r="G61" t="n">
-        <v>-0.17</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="62">
@@ -1866,16 +1866,16 @@
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>0.23</v>
+        <v>-0.23</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.79</v>
+        <v>0.79</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.87</v>
+        <v>0.87</v>
       </c>
       <c r="G62" t="n">
-        <v>1.89</v>
+        <v>-1.89</v>
       </c>
     </row>
     <row r="63">
@@ -1889,16 +1889,16 @@
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>2.08</v>
+        <v>-2.08</v>
       </c>
       <c r="E63" t="n">
-        <v>1.04</v>
+        <v>-1.04</v>
       </c>
       <c r="F63" t="n">
-        <v>1.02</v>
+        <v>-1.02</v>
       </c>
       <c r="G63" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="64">
@@ -1912,16 +1912,16 @@
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>1.38</v>
+        <v>-1.38</v>
       </c>
       <c r="E64" t="n">
-        <v>0.88</v>
+        <v>-0.88</v>
       </c>
       <c r="F64" t="n">
-        <v>0.97</v>
+        <v>-0.97</v>
       </c>
       <c r="G64" t="n">
-        <v>-0.47</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="65">
@@ -1935,16 +1935,16 @@
         <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>-3.42</v>
+        <v>3.42</v>
       </c>
       <c r="E65" t="n">
-        <v>-1.24</v>
+        <v>1.24</v>
       </c>
       <c r="F65" t="n">
-        <v>-1.16</v>
+        <v>1.16</v>
       </c>
       <c r="G65" t="n">
-        <v>-1.01</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="66">
@@ -1958,16 +1958,16 @@
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>-1.71</v>
+        <v>1.71</v>
       </c>
       <c r="E66" t="n">
-        <v>-0.64</v>
+        <v>0.64</v>
       </c>
       <c r="F66" t="n">
-        <v>-0.66</v>
+        <v>0.66</v>
       </c>
       <c r="G66" t="n">
-        <v>-0.41</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="67">
@@ -1981,16 +1981,16 @@
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>1.44</v>
+        <v>-1.44</v>
       </c>
       <c r="E67" t="n">
-        <v>0.76</v>
+        <v>-0.76</v>
       </c>
       <c r="F67" t="n">
-        <v>0.7</v>
+        <v>-0.7</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="68">
@@ -2004,16 +2004,16 @@
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>4.36</v>
+        <v>-4.36</v>
       </c>
       <c r="E68" t="n">
-        <v>1.41</v>
+        <v>-1.41</v>
       </c>
       <c r="F68" t="n">
-        <v>1.4</v>
+        <v>-1.4</v>
       </c>
       <c r="G68" t="n">
-        <v>1.55</v>
+        <v>-1.55</v>
       </c>
     </row>
     <row r="69">
@@ -2027,16 +2027,16 @@
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>1.63</v>
+        <v>-1.63</v>
       </c>
       <c r="E69" t="n">
-        <v>0.52</v>
+        <v>-0.52</v>
       </c>
       <c r="F69" t="n">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="G69" t="n">
-        <v>0.62</v>
+        <v>-0.62</v>
       </c>
     </row>
     <row r="70">
@@ -2050,16 +2050,16 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>1.22</v>
+        <v>-1.22</v>
       </c>
       <c r="E70" t="n">
-        <v>0.52</v>
+        <v>-0.52</v>
       </c>
       <c r="F70" t="n">
-        <v>0.54</v>
+        <v>-0.54</v>
       </c>
       <c r="G70" t="n">
-        <v>0.16</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="71">
@@ -2073,16 +2073,16 @@
         <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>-3.84</v>
+        <v>3.84</v>
       </c>
       <c r="E71" t="n">
-        <v>-1.37</v>
+        <v>1.37</v>
       </c>
       <c r="F71" t="n">
-        <v>-1.38</v>
+        <v>1.38</v>
       </c>
       <c r="G71" t="n">
-        <v>-1.09</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="72">
@@ -2096,16 +2096,16 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>-1.12</v>
+        <v>1.12</v>
       </c>
       <c r="E72" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.38</v>
+        <v>0.38</v>
       </c>
       <c r="G72" t="n">
-        <v>-0.29</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="73">
@@ -2119,16 +2119,16 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>-2.26</v>
+        <v>2.26</v>
       </c>
       <c r="E73" t="n">
-        <v>-0.63</v>
+        <v>0.63</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
       <c r="G73" t="n">
-        <v>-0.95</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="74">
@@ -2142,16 +2142,16 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>5.35</v>
+        <v>-5.35</v>
       </c>
       <c r="E74" t="n">
-        <v>1.69</v>
+        <v>-1.69</v>
       </c>
       <c r="F74" t="n">
-        <v>1.63</v>
+        <v>-1.63</v>
       </c>
       <c r="G74" t="n">
-        <v>2.02</v>
+        <v>-2.02</v>
       </c>
     </row>
     <row r="75">
@@ -2165,16 +2165,16 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.86</v>
+        <v>0.86</v>
       </c>
       <c r="E75" t="n">
-        <v>-0.38</v>
+        <v>0.38</v>
       </c>
       <c r="F75" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="G75" t="n">
-        <v>-0.48</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="76">
@@ -2188,16 +2188,16 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>-1.91</v>
+        <v>1.91</v>
       </c>
       <c r="E76" t="n">
-        <v>-0.67</v>
+        <v>0.67</v>
       </c>
       <c r="F76" t="n">
-        <v>-1.04</v>
+        <v>1.04</v>
       </c>
       <c r="G76" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="77">
@@ -2211,16 +2211,16 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>1.06</v>
+        <v>-1.06</v>
       </c>
       <c r="E77" t="n">
-        <v>0.71</v>
+        <v>-0.71</v>
       </c>
       <c r="F77" t="n">
-        <v>0.66</v>
+        <v>-0.66</v>
       </c>
       <c r="G77" t="n">
-        <v>-0.31</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="78">
@@ -2234,16 +2234,16 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>-1.57</v>
+        <v>1.57</v>
       </c>
       <c r="E78" t="n">
-        <v>-0.43</v>
+        <v>0.43</v>
       </c>
       <c r="F78" t="n">
-        <v>-0.71</v>
+        <v>0.71</v>
       </c>
       <c r="G78" t="n">
-        <v>-0.44</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="79">
@@ -2257,16 +2257,16 @@
         <v>1</v>
       </c>
       <c r="D79" t="n">
-        <v>-2.07</v>
+        <v>2.07</v>
       </c>
       <c r="E79" t="n">
-        <v>-0.92</v>
+        <v>0.92</v>
       </c>
       <c r="F79" t="n">
-        <v>-0.56</v>
+        <v>0.56</v>
       </c>
       <c r="G79" t="n">
-        <v>-0.59</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="80">
@@ -2280,16 +2280,16 @@
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>2.25</v>
+        <v>-2.25</v>
       </c>
       <c r="E80" t="n">
-        <v>-0.05</v>
+        <v>0.05</v>
       </c>
       <c r="F80" t="n">
-        <v>0.46</v>
+        <v>-0.46</v>
       </c>
       <c r="G80" t="n">
-        <v>1.84</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="81">
@@ -2303,16 +2303,16 @@
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>3.92</v>
+        <v>-3.92</v>
       </c>
       <c r="E81" t="n">
-        <v>1.99</v>
+        <v>-1.99</v>
       </c>
       <c r="F81" t="n">
-        <v>1.47</v>
+        <v>-1.47</v>
       </c>
       <c r="G81" t="n">
-        <v>0.46</v>
+        <v>-0.46</v>
       </c>
     </row>
     <row r="82">
@@ -2326,16 +2326,16 @@
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.07</v>
+        <v>-0.07</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="F82" t="n">
-        <v>0.63</v>
+        <v>-0.63</v>
       </c>
       <c r="G82" t="n">
-        <v>-0.36</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="83">
@@ -2349,16 +2349,16 @@
         <v>1</v>
       </c>
       <c r="D83" t="n">
-        <v>-2.25</v>
+        <v>2.25</v>
       </c>
       <c r="E83" t="n">
-        <v>-0.64</v>
+        <v>0.64</v>
       </c>
       <c r="F83" t="n">
-        <v>-0.91</v>
+        <v>0.91</v>
       </c>
       <c r="G83" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="84">
@@ -2372,16 +2372,16 @@
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>-2.08</v>
+        <v>2.08</v>
       </c>
       <c r="E84" t="n">
-        <v>-0.59</v>
+        <v>0.59</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.92</v>
+        <v>0.92</v>
       </c>
       <c r="G84" t="n">
-        <v>-0.57</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="85">
@@ -2395,16 +2395,16 @@
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>-1.91</v>
+        <v>1.91</v>
       </c>
       <c r="E85" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="F85" t="n">
-        <v>-0.74</v>
+        <v>0.74</v>
       </c>
       <c r="G85" t="n">
-        <v>-0.67</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="86">
@@ -2418,16 +2418,16 @@
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>2.95</v>
+        <v>-2.95</v>
       </c>
       <c r="E86" t="n">
-        <v>0.76</v>
+        <v>-0.76</v>
       </c>
       <c r="F86" t="n">
-        <v>0.89</v>
+        <v>-0.89</v>
       </c>
       <c r="G86" t="n">
-        <v>1.3</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="87">
@@ -2441,16 +2441,16 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.13</v>
+        <v>0.13</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
       <c r="G87" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="88">
@@ -2464,16 +2464,16 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>-2.27</v>
+        <v>2.27</v>
       </c>
       <c r="E88" t="n">
-        <v>-0.69</v>
+        <v>0.69</v>
       </c>
       <c r="F88" t="n">
-        <v>-0.78</v>
+        <v>0.78</v>
       </c>
       <c r="G88" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="89">
@@ -2487,16 +2487,16 @@
         <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>-2.84</v>
+        <v>2.84</v>
       </c>
       <c r="E89" t="n">
-        <v>-0.94</v>
+        <v>0.94</v>
       </c>
       <c r="F89" t="n">
-        <v>-0.93</v>
+        <v>0.93</v>
       </c>
       <c r="G89" t="n">
-        <v>-0.97</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="90">
@@ -2510,16 +2510,16 @@
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>-1.98</v>
+        <v>1.98</v>
       </c>
       <c r="E90" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F90" t="n">
-        <v>-0.57</v>
+        <v>0.57</v>
       </c>
       <c r="G90" t="n">
-        <v>-0.69</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="91">
@@ -2533,16 +2533,16 @@
         <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>4.27</v>
+        <v>-4.27</v>
       </c>
       <c r="E91" t="n">
-        <v>1.6</v>
+        <v>-1.6</v>
       </c>
       <c r="F91" t="n">
-        <v>1.54</v>
+        <v>-1.54</v>
       </c>
       <c r="G91" t="n">
-        <v>1.13</v>
+        <v>-1.13</v>
       </c>
     </row>
     <row r="92">
@@ -2556,16 +2556,16 @@
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>0.87</v>
+        <v>-0.87</v>
       </c>
       <c r="E92" t="n">
-        <v>-0.54</v>
+        <v>0.54</v>
       </c>
       <c r="F92" t="n">
-        <v>-0.63</v>
+        <v>0.63</v>
       </c>
       <c r="G92" t="n">
-        <v>2.03</v>
+        <v>-2.03</v>
       </c>
     </row>
     <row r="93">
@@ -2579,16 +2579,16 @@
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>2.32</v>
+        <v>-2.32</v>
       </c>
       <c r="E93" t="n">
-        <v>1.2</v>
+        <v>-1.2</v>
       </c>
       <c r="F93" t="n">
-        <v>1.54</v>
+        <v>-1.54</v>
       </c>
       <c r="G93" t="n">
-        <v>-0.42</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="94">
@@ -2602,16 +2602,16 @@
         <v>1</v>
       </c>
       <c r="D94" t="n">
-        <v>-2.13</v>
+        <v>2.13</v>
       </c>
       <c r="E94" t="n">
-        <v>-1.05</v>
+        <v>1.05</v>
       </c>
       <c r="F94" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
       <c r="G94" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="95">
@@ -2625,16 +2625,16 @@
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>-1.95</v>
+        <v>1.95</v>
       </c>
       <c r="E95" t="n">
-        <v>-0.97</v>
+        <v>0.97</v>
       </c>
       <c r="F95" t="n">
-        <v>-0.67</v>
+        <v>0.67</v>
       </c>
       <c r="G95" t="n">
-        <v>-0.3</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="96">
@@ -2648,16 +2648,16 @@
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
       <c r="E96" t="n">
-        <v>0.31</v>
+        <v>-0.31</v>
       </c>
       <c r="F96" t="n">
-        <v>-0.56</v>
+        <v>0.56</v>
       </c>
       <c r="G96" t="n">
-        <v>-0.55</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="97">
@@ -2671,16 +2671,16 @@
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>1.69</v>
+        <v>-1.69</v>
       </c>
       <c r="E97" t="n">
-        <v>1.06</v>
+        <v>-1.06</v>
       </c>
       <c r="F97" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G97" t="n">
-        <v>-0.37</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="98">
@@ -2694,16 +2694,16 @@
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>1.74</v>
+        <v>-1.74</v>
       </c>
       <c r="E98" t="n">
-        <v>-0.08</v>
+        <v>0.08</v>
       </c>
       <c r="F98" t="n">
-        <v>-0.16</v>
+        <v>0.16</v>
       </c>
       <c r="G98" t="n">
-        <v>1.98</v>
+        <v>-1.98</v>
       </c>
     </row>
     <row r="99">
@@ -2717,16 +2717,16 @@
         <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>-1.05</v>
+        <v>1.05</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.49</v>
+        <v>0.49</v>
       </c>
       <c r="F99" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
       <c r="G99" t="n">
-        <v>-0.16</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="100">
@@ -2740,16 +2740,16 @@
         <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>-1.15</v>
+        <v>1.15</v>
       </c>
       <c r="E100" t="n">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="F100" t="n">
-        <v>-0.36</v>
+        <v>0.36</v>
       </c>
       <c r="G100" t="n">
-        <v>-0.55</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="101">
@@ -2763,16 +2763,16 @@
         <v>1</v>
       </c>
       <c r="D101" t="n">
-        <v>-2.06</v>
+        <v>2.06</v>
       </c>
       <c r="E101" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F101" t="n">
-        <v>-0.66</v>
+        <v>0.66</v>
       </c>
       <c r="G101" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="102">
@@ -2786,16 +2786,16 @@
         <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>-1.42</v>
+        <v>1.42</v>
       </c>
       <c r="E102" t="n">
-        <v>-0.46</v>
+        <v>0.46</v>
       </c>
       <c r="F102" t="n">
-        <v>-0.43</v>
+        <v>0.43</v>
       </c>
       <c r="G102" t="n">
-        <v>-0.53</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="103">
@@ -2809,16 +2809,16 @@
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>3.93</v>
+        <v>-3.93</v>
       </c>
       <c r="E103" t="n">
-        <v>1.99</v>
+        <v>-1.99</v>
       </c>
       <c r="F103" t="n">
-        <v>2.02</v>
+        <v>-2.02</v>
       </c>
       <c r="G103" t="n">
-        <v>-0.07</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="104">
@@ -2832,16 +2832,16 @@
         <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>1.73</v>
+        <v>-1.73</v>
       </c>
       <c r="E104" t="n">
-        <v>-0.29</v>
+        <v>0.29</v>
       </c>
       <c r="F104" t="n">
-        <v>0.26</v>
+        <v>-0.26</v>
       </c>
       <c r="G104" t="n">
-        <v>1.76</v>
+        <v>-1.76</v>
       </c>
     </row>
     <row r="105">
@@ -2855,16 +2855,16 @@
         <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="E105" t="n">
-        <v>2.01</v>
+        <v>-2.01</v>
       </c>
       <c r="F105" t="n">
-        <v>1.45</v>
+        <v>-1.45</v>
       </c>
       <c r="G105" t="n">
-        <v>0.54</v>
+        <v>-0.54</v>
       </c>
     </row>
     <row r="106">
@@ -2878,16 +2878,16 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.41</v>
+        <v>-0.41</v>
       </c>
       <c r="E106" t="n">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
       <c r="F106" t="n">
-        <v>0.7</v>
+        <v>-0.7</v>
       </c>
       <c r="G106" t="n">
-        <v>-0.13</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="107">
@@ -2901,16 +2901,16 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>-1.49</v>
+        <v>1.49</v>
       </c>
       <c r="E107" t="n">
-        <v>-0.47</v>
+        <v>0.47</v>
       </c>
       <c r="F107" t="n">
-        <v>-0.43</v>
+        <v>0.43</v>
       </c>
       <c r="G107" t="n">
-        <v>-0.59</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="108">
@@ -2924,16 +2924,16 @@
         <v>1</v>
       </c>
       <c r="D108" t="n">
-        <v>-2.72</v>
+        <v>2.72</v>
       </c>
       <c r="E108" t="n">
-        <v>-0.53</v>
+        <v>0.53</v>
       </c>
       <c r="F108" t="n">
-        <v>-1.3</v>
+        <v>1.3</v>
       </c>
       <c r="G108" t="n">
-        <v>-0.89</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="109">
@@ -2947,16 +2947,16 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>-1.93</v>
+        <v>1.93</v>
       </c>
       <c r="E109" t="n">
-        <v>-0.58</v>
+        <v>0.58</v>
       </c>
       <c r="F109" t="n">
-        <v>-0.67</v>
+        <v>0.67</v>
       </c>
       <c r="G109" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="110">
@@ -2970,16 +2970,16 @@
         <v>1</v>
       </c>
       <c r="D110" t="n">
-        <v>-2.25</v>
+        <v>2.25</v>
       </c>
       <c r="E110" t="n">
-        <v>-0.86</v>
+        <v>0.86</v>
       </c>
       <c r="F110" t="n">
-        <v>-0.73</v>
+        <v>0.73</v>
       </c>
       <c r="G110" t="n">
-        <v>-0.66</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="111">
@@ -2993,16 +2993,16 @@
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
       <c r="E111" t="n">
-        <v>-0.09</v>
+        <v>0.09</v>
       </c>
       <c r="F111" t="n">
-        <v>-0.43</v>
+        <v>0.43</v>
       </c>
       <c r="G111" t="n">
-        <v>-0.28</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="112">
@@ -3016,16 +3016,16 @@
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>-0.29</v>
+        <v>0.29</v>
       </c>
       <c r="E112" t="n">
-        <v>-0.16</v>
+        <v>0.16</v>
       </c>
       <c r="F112" t="n">
-        <v>0.22</v>
+        <v>-0.22</v>
       </c>
       <c r="G112" t="n">
-        <v>-0.35</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="113">
@@ -3039,16 +3039,16 @@
         <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>-2.18</v>
+        <v>2.18</v>
       </c>
       <c r="E113" t="n">
-        <v>-0.79</v>
+        <v>0.79</v>
       </c>
       <c r="F113" t="n">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="G113" t="n">
-        <v>-0.63</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="114">
@@ -3062,16 +3062,16 @@
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>-0.27</v>
+        <v>0.27</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
       </c>
       <c r="F114" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="G114" t="n">
-        <v>-0.06</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="115">
@@ -3085,16 +3085,16 @@
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>5.79</v>
+        <v>-5.79</v>
       </c>
       <c r="E115" t="n">
-        <v>1.9</v>
+        <v>-1.9</v>
       </c>
       <c r="F115" t="n">
-        <v>1.9</v>
+        <v>-1.9</v>
       </c>
       <c r="G115" t="n">
-        <v>1.99</v>
+        <v>-1.99</v>
       </c>
     </row>
     <row r="116">
@@ -3125,16 +3125,16 @@
         <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>-0.27</v>
+        <v>0.27</v>
       </c>
       <c r="E117" t="n">
-        <v>-0.94</v>
+        <v>0.94</v>
       </c>
       <c r="F117" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="G117" t="n">
-        <v>1.12</v>
+        <v>-1.12</v>
       </c>
     </row>
     <row r="118">
@@ -3148,13 +3148,13 @@
         <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>0.62</v>
+        <v>-0.62</v>
       </c>
       <c r="E118" t="n">
-        <v>1.06</v>
+        <v>-1.06</v>
       </c>
       <c r="F118" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="G118"/>
     </row>
@@ -3169,16 +3169,16 @@
         <v>0</v>
       </c>
       <c r="D119" t="n">
-        <v>2.34</v>
+        <v>-2.34</v>
       </c>
       <c r="E119" t="n">
-        <v>1.06</v>
+        <v>-1.06</v>
       </c>
       <c r="F119" t="n">
-        <v>1.79</v>
+        <v>-1.79</v>
       </c>
       <c r="G119" t="n">
-        <v>-0.51</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="120">
@@ -3192,16 +3192,16 @@
         <v>1</v>
       </c>
       <c r="D120" t="n">
-        <v>-2.43</v>
+        <v>2.43</v>
       </c>
       <c r="E120" t="n">
-        <v>-0.88</v>
+        <v>0.88</v>
       </c>
       <c r="F120" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="G120" t="n">
-        <v>-1.11</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="121">
@@ -3215,16 +3215,16 @@
         <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>-0.26</v>
+        <v>0.26</v>
       </c>
       <c r="E121" t="n">
-        <v>-0.31</v>
+        <v>0.31</v>
       </c>
       <c r="F121" t="n">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
       <c r="G121" t="n">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="122">
@@ -3238,16 +3238,16 @@
         <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>-1.37</v>
+        <v>1.37</v>
       </c>
       <c r="E122" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F122" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="G122" t="n">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="123">
@@ -3261,16 +3261,16 @@
         <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>0.76</v>
+        <v>-0.76</v>
       </c>
       <c r="E123" t="n">
-        <v>1.15</v>
+        <v>-1.15</v>
       </c>
       <c r="F123" t="n">
-        <v>-0.09</v>
+        <v>0.09</v>
       </c>
       <c r="G123" t="n">
-        <v>-0.3</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="124">
@@ -3284,16 +3284,16 @@
         <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>-1.62</v>
+        <v>1.62</v>
       </c>
       <c r="E124" t="n">
-        <v>-0.62</v>
+        <v>0.62</v>
       </c>
       <c r="F124" t="n">
-        <v>-0.48</v>
+        <v>0.48</v>
       </c>
       <c r="G124" t="n">
-        <v>-0.52</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="125">
@@ -3307,16 +3307,16 @@
         <v>1</v>
       </c>
       <c r="D125" t="n">
-        <v>-1.66</v>
+        <v>1.66</v>
       </c>
       <c r="E125" t="n">
-        <v>-0.65</v>
+        <v>0.65</v>
       </c>
       <c r="F125" t="n">
-        <v>-0.49</v>
+        <v>0.49</v>
       </c>
       <c r="G125" t="n">
-        <v>-0.52</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="126">
@@ -3330,16 +3330,16 @@
         <v>0</v>
       </c>
       <c r="D126" t="n">
-        <v>-1.56</v>
+        <v>1.56</v>
       </c>
       <c r="E126" t="n">
-        <v>-0.58</v>
+        <v>0.58</v>
       </c>
       <c r="F126" t="n">
-        <v>-0.46</v>
+        <v>0.46</v>
       </c>
       <c r="G126" t="n">
-        <v>-0.52</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="127">
@@ -3353,16 +3353,16 @@
         <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>5.45</v>
+        <v>-5.45</v>
       </c>
       <c r="E127" t="n">
-        <v>1.42</v>
+        <v>-1.42</v>
       </c>
       <c r="F127" t="n">
-        <v>2.02</v>
+        <v>-2.02</v>
       </c>
       <c r="G127" t="n">
-        <v>2.02</v>
+        <v>-2.02</v>
       </c>
     </row>
     <row r="128">
@@ -3376,16 +3376,16 @@
         <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>3.66</v>
+        <v>-3.66</v>
       </c>
       <c r="E128" t="n">
-        <v>1.84</v>
+        <v>-1.84</v>
       </c>
       <c r="F128" t="n">
-        <v>1.99</v>
+        <v>-1.99</v>
       </c>
       <c r="G128" t="n">
-        <v>-0.16</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="129">
@@ -3399,16 +3399,16 @@
         <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>-1.66</v>
+        <v>1.66</v>
       </c>
       <c r="E129" t="n">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="F129" t="n">
-        <v>-0.61</v>
+        <v>0.61</v>
       </c>
       <c r="G129" t="n">
-        <v>-0.32</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="130">
@@ -3422,16 +3422,16 @@
         <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>-1.77</v>
+        <v>1.77</v>
       </c>
       <c r="E130" t="n">
-        <v>-0.61</v>
+        <v>0.61</v>
       </c>
       <c r="F130" t="n">
-        <v>-0.37</v>
+        <v>0.37</v>
       </c>
       <c r="G130" t="n">
-        <v>-0.79</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="131">
@@ -3445,16 +3445,16 @@
         <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
       <c r="E131" t="n">
-        <v>-0.35</v>
+        <v>0.35</v>
       </c>
       <c r="F131" t="n">
-        <v>-0.49</v>
+        <v>0.49</v>
       </c>
       <c r="G131" t="n">
-        <v>0.15</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="132">
@@ -3468,16 +3468,16 @@
         <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>2.41</v>
+        <v>-2.41</v>
       </c>
       <c r="E132" t="n">
-        <v>0.47</v>
+        <v>-0.47</v>
       </c>
       <c r="F132" t="n">
-        <v>0.04</v>
+        <v>-0.04</v>
       </c>
       <c r="G132" t="n">
-        <v>1.9</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="133">
@@ -3491,16 +3491,16 @@
         <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>-1.95</v>
+        <v>1.95</v>
       </c>
       <c r="E133" t="n">
-        <v>-0.62</v>
+        <v>0.62</v>
       </c>
       <c r="F133" t="n">
-        <v>-0.55</v>
+        <v>0.55</v>
       </c>
       <c r="G133" t="n">
-        <v>-0.78</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="134">
@@ -3514,16 +3514,16 @@
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>1.41</v>
+        <v>-1.41</v>
       </c>
       <c r="E134" t="n">
-        <v>-0.44</v>
+        <v>0.44</v>
       </c>
       <c r="F134" t="n">
-        <v>-0.13</v>
+        <v>0.13</v>
       </c>
       <c r="G134" t="n">
-        <v>1.97</v>
+        <v>-1.97</v>
       </c>
     </row>
     <row r="135">
@@ -3537,16 +3537,16 @@
         <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>-0.27</v>
+        <v>0.27</v>
       </c>
       <c r="E135" t="n">
-        <v>0.45</v>
+        <v>-0.45</v>
       </c>
       <c r="F135" t="n">
-        <v>-0.06</v>
+        <v>0.06</v>
       </c>
       <c r="G135" t="n">
-        <v>-0.66</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="136">
@@ -3560,16 +3560,16 @@
         <v>1</v>
       </c>
       <c r="D136" t="n">
-        <v>-1.89</v>
+        <v>1.89</v>
       </c>
       <c r="E136" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
       <c r="F136" t="n">
-        <v>-0.51</v>
+        <v>0.51</v>
       </c>
       <c r="G136" t="n">
-        <v>-0.69</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="137">
@@ -3583,16 +3583,16 @@
         <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>-1.59</v>
+        <v>1.59</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.63</v>
+        <v>0.63</v>
       </c>
       <c r="F137" t="n">
-        <v>-0.68</v>
+        <v>0.68</v>
       </c>
       <c r="G137" t="n">
-        <v>-0.29</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="138">
@@ -3606,16 +3606,16 @@
         <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>-1.51</v>
+        <v>1.51</v>
       </c>
       <c r="E138" t="n">
-        <v>-0.56</v>
+        <v>0.56</v>
       </c>
       <c r="F138" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="G138" t="n">
-        <v>-0.35</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="139">
@@ -3629,16 +3629,16 @@
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>3.85</v>
+        <v>-3.85</v>
       </c>
       <c r="E139" t="n">
-        <v>1.85</v>
+        <v>-1.85</v>
       </c>
       <c r="F139" t="n">
-        <v>1.97</v>
+        <v>-1.97</v>
       </c>
       <c r="G139" t="n">
-        <v>0.02</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="140">
@@ -3652,16 +3652,16 @@
         <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>3.33</v>
+        <v>-3.33</v>
       </c>
       <c r="E140" t="n">
-        <v>0.98</v>
+        <v>-0.98</v>
       </c>
       <c r="F140" t="n">
-        <v>0.85</v>
+        <v>-0.85</v>
       </c>
       <c r="G140" t="n">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="141">
@@ -3675,16 +3675,16 @@
         <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>-0.47</v>
+        <v>0.47</v>
       </c>
       <c r="E141" t="n">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="F141" t="n">
-        <v>-0.22</v>
+        <v>0.22</v>
       </c>
       <c r="G141" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="142">
@@ -3698,13 +3698,13 @@
         <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>1.83</v>
+        <v>-1.83</v>
       </c>
       <c r="E142" t="n">
-        <v>0.98</v>
+        <v>-0.98</v>
       </c>
       <c r="F142" t="n">
-        <v>0.85</v>
+        <v>-0.85</v>
       </c>
       <c r="G142"/>
     </row>
@@ -3719,13 +3719,13 @@
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>0.97</v>
+        <v>-0.97</v>
       </c>
       <c r="E143" t="n">
-        <v>0.13</v>
+        <v>-0.13</v>
       </c>
       <c r="F143" t="n">
-        <v>0.84</v>
+        <v>-0.84</v>
       </c>
       <c r="G143"/>
     </row>
@@ -3740,16 +3740,16 @@
         <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>-3.4</v>
+        <v>3.4</v>
       </c>
       <c r="E144" t="n">
-        <v>-1.53</v>
+        <v>1.53</v>
       </c>
       <c r="F144" t="n">
-        <v>-1.37</v>
+        <v>1.37</v>
       </c>
       <c r="G144" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="145">
@@ -3763,16 +3763,16 @@
         <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>-2.27</v>
+        <v>2.27</v>
       </c>
       <c r="E145" t="n">
-        <v>-0.81</v>
+        <v>0.81</v>
       </c>
       <c r="F145" t="n">
-        <v>-0.96</v>
+        <v>0.96</v>
       </c>
       <c r="G145" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with 0.1 smoothing
</commit_message>
<xml_diff>
--- a/outcome/appendix/Figure Data/Fig.3 data.xlsx
+++ b/outcome/appendix/Figure Data/Fig.3 data.xlsx
@@ -488,16 +488,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.19</v>
+        <v>-0.21</v>
       </c>
       <c r="E2" t="n">
         <v>0.14</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.35</v>
+        <v>-0.32</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="3">
@@ -511,16 +511,16 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="E3" t="n">
         <v>-0.11</v>
       </c>
       <c r="F3" t="n">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
       <c r="G3" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="4">
@@ -534,16 +534,16 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.83</v>
+        <v>0.71</v>
       </c>
       <c r="E4" t="n">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="F4" t="n">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="G4" t="n">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5">
@@ -554,19 +554,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.53</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.11</v>
       </c>
     </row>
     <row r="6">
@@ -577,19 +577,19 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>2.18</v>
+        <v>2.55</v>
       </c>
       <c r="E6" t="n">
-        <v>0.74</v>
+        <v>0.77</v>
       </c>
       <c r="F6" t="n">
-        <v>0.93</v>
+        <v>1.03</v>
       </c>
       <c r="G6" t="n">
-        <v>0.51</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7">
@@ -603,16 +603,16 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-5.62</v>
+        <v>-5.58</v>
       </c>
       <c r="E7" t="n">
         <v>-1.93</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.82</v>
+        <v>-1.8</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.87</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="8">
@@ -626,16 +626,16 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.03</v>
+        <v>0.94</v>
       </c>
       <c r="E8" t="n">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="F8" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="G8" t="n">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="9">
@@ -649,16 +649,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.84</v>
+        <v>1.78</v>
       </c>
       <c r="E9" t="n">
-        <v>0.72</v>
+        <v>0.69</v>
       </c>
       <c r="F9" t="n">
-        <v>0.58</v>
+        <v>0.56</v>
       </c>
       <c r="G9" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="10">
@@ -672,16 +672,16 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.79</v>
+        <v>-1.84</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.63</v>
+        <v>-0.65</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.52</v>
+        <v>-0.53</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.64</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>3.27</v>
+        <v>3.18</v>
       </c>
       <c r="E11" t="n">
-        <v>1.16</v>
+        <v>1.11</v>
       </c>
       <c r="F11" t="n">
-        <v>1.06</v>
+        <v>1.03</v>
       </c>
       <c r="G11" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="12">
@@ -718,16 +718,16 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.73</v>
+        <v>1.05</v>
       </c>
       <c r="E12" t="n">
-        <v>0.14</v>
+        <v>0.29</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="13">
@@ -741,16 +741,16 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-5.09</v>
+        <v>-5.12</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.64</v>
+        <v>-1.65</v>
       </c>
       <c r="F13" t="n">
-        <v>-1.75</v>
+        <v>-1.76</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.7</v>
+        <v>-1.71</v>
       </c>
     </row>
     <row r="14">
@@ -902,16 +902,16 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.16</v>
+        <v>-0.31</v>
       </c>
       <c r="E20" t="n">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="F20" t="n">
-        <v>0.81</v>
+        <v>0.79</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.69</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="21">
@@ -925,16 +925,16 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-2.15</v>
+        <v>-2.36</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.42</v>
+        <v>-1.48</v>
       </c>
       <c r="F21" t="n">
-        <v>-1.13</v>
+        <v>-1.14</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="22">
@@ -948,16 +948,16 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.51</v>
+        <v>0.74</v>
       </c>
       <c r="E22" t="n">
-        <v>0.44</v>
+        <v>0.47</v>
       </c>
       <c r="F22" t="n">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.09</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="23">
@@ -971,16 +971,16 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.99</v>
+        <v>1.13</v>
       </c>
       <c r="E23" t="n">
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
       <c r="F23" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.47</v>
+        <v>-0.29</v>
       </c>
     </row>
     <row r="24">
@@ -994,16 +994,16 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>2.25</v>
+        <v>2.22</v>
       </c>
       <c r="E24" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="F24" t="n">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
       <c r="G24" t="n">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="25">
@@ -1017,16 +1017,16 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-1.44</v>
+        <v>-1.42</v>
       </c>
       <c r="E25" t="n">
-        <v>-1.13</v>
+        <v>-1.07</v>
       </c>
       <c r="F25" t="n">
         <v>-1.37</v>
       </c>
       <c r="G25" t="n">
-        <v>1.07</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="26">
@@ -1040,16 +1040,16 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-5.71</v>
+        <v>-5.42</v>
       </c>
       <c r="E26" t="n">
-        <v>-1.99</v>
+        <v>-1.91</v>
       </c>
       <c r="F26" t="n">
-        <v>-1.72</v>
+        <v>-1.5</v>
       </c>
       <c r="G26" t="n">
-        <v>-2.01</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="27">
@@ -1063,16 +1063,16 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>1.57</v>
+        <v>1.44</v>
       </c>
       <c r="E27" t="n">
-        <v>0.43</v>
+        <v>0.39</v>
       </c>
       <c r="F27" t="n">
-        <v>0.6</v>
+        <v>0.47</v>
       </c>
       <c r="G27" t="n">
-        <v>0.55</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="28">
@@ -1086,16 +1086,16 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.06</v>
+        <v>0.02</v>
       </c>
       <c r="G28" t="n">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="29">
@@ -1109,16 +1109,16 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.88</v>
+        <v>0.51</v>
       </c>
       <c r="E29" t="n">
-        <v>0.29</v>
+        <v>0.18</v>
       </c>
       <c r="F29" t="n">
-        <v>0.26</v>
+        <v>0.05</v>
       </c>
       <c r="G29" t="n">
-        <v>0.33</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="30">
@@ -1132,16 +1132,16 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>2.39</v>
+        <v>2.96</v>
       </c>
       <c r="E30" t="n">
-        <v>0.79</v>
+        <v>1.01</v>
       </c>
       <c r="F30" t="n">
-        <v>1.24</v>
+        <v>1.49</v>
       </c>
       <c r="G30" t="n">
-        <v>0.36</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="31">
@@ -1155,16 +1155,16 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.08</v>
+        <v>-0.49</v>
       </c>
       <c r="E31" t="n">
-        <v>0.08</v>
+        <v>-0.04</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.32</v>
+        <v>-0.54</v>
       </c>
       <c r="G31" t="n">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="32">
@@ -1178,13 +1178,13 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.48</v>
+        <v>-0.34</v>
       </c>
       <c r="E32" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="F32" t="n">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
         <v>-1.91</v>
@@ -1201,16 +1201,16 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>1.55</v>
+        <v>1.7</v>
       </c>
       <c r="E33" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="F33" t="n">
-        <v>0.55</v>
+        <v>0.68</v>
       </c>
       <c r="G33" t="n">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="34">
@@ -1224,16 +1224,16 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>2.19</v>
+        <v>1.87</v>
       </c>
       <c r="E34" t="n">
-        <v>0.98</v>
+        <v>0.92</v>
       </c>
       <c r="F34" t="n">
-        <v>0.84</v>
+        <v>0.59</v>
       </c>
       <c r="G34" t="n">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="35">
@@ -1247,13 +1247,13 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>-2.11</v>
+        <v>-2.09</v>
       </c>
       <c r="E35" t="n">
         <v>-0.88</v>
       </c>
       <c r="F35" t="n">
-        <v>-1.16</v>
+        <v>-1.15</v>
       </c>
       <c r="G35" t="n">
         <v>-0.06</v>
@@ -1270,10 +1270,10 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="E36" t="n">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
       <c r="F36" t="n">
         <v>0.23</v>
@@ -1293,16 +1293,16 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>-2.17</v>
+        <v>-2.18</v>
       </c>
       <c r="E37" t="n">
-        <v>-1.55</v>
+        <v>-1.56</v>
       </c>
       <c r="F37" t="n">
         <v>-1.34</v>
       </c>
       <c r="G37" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="38">
@@ -1316,16 +1316,16 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>2.1</v>
+        <v>2.07</v>
       </c>
       <c r="E38" t="n">
-        <v>0.75</v>
+        <v>0.77</v>
       </c>
       <c r="F38" t="n">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
       <c r="G38" t="n">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="39">
@@ -1342,13 +1342,13 @@
         <v>-0.89</v>
       </c>
       <c r="E39" t="n">
-        <v>-1.51</v>
+        <v>-1.5</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.82</v>
+        <v>-0.81</v>
       </c>
       <c r="G39" t="n">
-        <v>1.45</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="40">
@@ -1362,16 +1362,16 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.54</v>
+        <v>-0.65</v>
       </c>
       <c r="E40" t="n">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="F40" t="n">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.38</v>
+        <v>-1.45</v>
       </c>
     </row>
     <row r="41">
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>1.46</v>
+        <v>1.51</v>
       </c>
       <c r="E41" t="n">
         <v>0.76</v>
@@ -1394,7 +1394,7 @@
         <v>0.9</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.2</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="42">
@@ -1408,16 +1408,16 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.69</v>
+        <v>0.76</v>
       </c>
       <c r="E42" t="n">
         <v>0.57</v>
       </c>
       <c r="F42" t="n">
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.52</v>
+        <v>-0.48</v>
       </c>
     </row>
     <row r="43">
@@ -1431,16 +1431,16 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>-2.82</v>
+        <v>-2.79</v>
       </c>
       <c r="E43" t="n">
-        <v>-1.02</v>
+        <v>-1.04</v>
       </c>
       <c r="F43" t="n">
         <v>-1.64</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.16</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="44">
@@ -1454,16 +1454,16 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>-4.18</v>
+        <v>-4.82</v>
       </c>
       <c r="E44" t="n">
-        <v>-1.8</v>
+        <v>-1.85</v>
       </c>
       <c r="F44" t="n">
-        <v>-1.72</v>
+        <v>-1.76</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.66</v>
+        <v>-1.21</v>
       </c>
     </row>
     <row r="45">
@@ -1477,16 +1477,16 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1.43</v>
+        <v>0.94</v>
       </c>
       <c r="E45" t="n">
-        <v>0.48</v>
+        <v>0.28</v>
       </c>
       <c r="F45" t="n">
-        <v>0.43</v>
+        <v>0.29</v>
       </c>
       <c r="G45" t="n">
-        <v>0.52</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="46">
@@ -1500,16 +1500,16 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1.98</v>
+        <v>1.86</v>
       </c>
       <c r="E46" t="n">
-        <v>0.66</v>
+        <v>0.55</v>
       </c>
       <c r="F46" t="n">
-        <v>0.61</v>
+        <v>0.54</v>
       </c>
       <c r="G46" t="n">
-        <v>0.72</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="47">
@@ -1523,13 +1523,13 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.7</v>
+        <v>-0.88</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.28</v>
+        <v>-0.38</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.42</v>
+        <v>-0.5</v>
       </c>
       <c r="G47"/>
     </row>
@@ -1544,16 +1544,16 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.53</v>
+        <v>-0.04</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.06</v>
+        <v>0.51</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.04</v>
+        <v>0.36</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.43</v>
+        <v>-0.91</v>
       </c>
     </row>
     <row r="49">
@@ -1567,16 +1567,16 @@
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>3</v>
+        <v>2.94</v>
       </c>
       <c r="E49" t="n">
-        <v>1.01</v>
+        <v>0.89</v>
       </c>
       <c r="F49" t="n">
-        <v>1.14</v>
+        <v>1.07</v>
       </c>
       <c r="G49" t="n">
-        <v>0.85</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="50">
@@ -1590,16 +1590,16 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>-4.19</v>
+        <v>-4.02</v>
       </c>
       <c r="E50" t="n">
-        <v>-1.42</v>
+        <v>-1.37</v>
       </c>
       <c r="F50" t="n">
-        <v>-1.47</v>
+        <v>-1.41</v>
       </c>
       <c r="G50" t="n">
-        <v>-1.3</v>
+        <v>-1.23</v>
       </c>
     </row>
     <row r="51">
@@ -1613,16 +1613,16 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>-3.46</v>
+        <v>-3.64</v>
       </c>
       <c r="E51" t="n">
-        <v>-1.13</v>
+        <v>-1.19</v>
       </c>
       <c r="F51" t="n">
-        <v>-1.08</v>
+        <v>-1.14</v>
       </c>
       <c r="G51" t="n">
-        <v>-1.25</v>
+        <v>-1.32</v>
       </c>
     </row>
     <row r="52">
@@ -1636,16 +1636,16 @@
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>1.63</v>
+        <v>1.6</v>
       </c>
       <c r="E52" t="n">
-        <v>0.56</v>
+        <v>0.55</v>
       </c>
       <c r="F52" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="G52" t="n">
-        <v>0.56</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="53">
@@ -1659,13 +1659,13 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>1.86</v>
+        <v>1.87</v>
       </c>
       <c r="E53" t="n">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="F53" t="n">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="G53" t="n">
         <v>0.92</v>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>2.07</v>
+        <v>2.09</v>
       </c>
       <c r="E54" t="n">
         <v>0.75</v>
@@ -1691,7 +1691,7 @@
         <v>0.76</v>
       </c>
       <c r="G54" t="n">
-        <v>0.56</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="55">
@@ -1705,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>2.09</v>
+        <v>2.1</v>
       </c>
       <c r="E55" t="n">
         <v>0.79</v>
@@ -1728,16 +1728,16 @@
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>-4.25</v>
+        <v>-3.84</v>
       </c>
       <c r="E56" t="n">
-        <v>-1.63</v>
+        <v>-1.45</v>
       </c>
       <c r="F56" t="n">
-        <v>-1.81</v>
+        <v>-1.66</v>
       </c>
       <c r="G56" t="n">
-        <v>-0.81</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="57">
@@ -1751,16 +1751,16 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>-1.59</v>
+        <v>-1.04</v>
       </c>
       <c r="E57" t="n">
-        <v>-0.28</v>
+        <v>-0.06</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.03</v>
+        <v>0.12</v>
       </c>
       <c r="G57" t="n">
-        <v>-1.28</v>
+        <v>-1.1</v>
       </c>
     </row>
     <row r="58">
@@ -1774,16 +1774,16 @@
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.74</v>
+        <v>-1.94</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.51</v>
+        <v>-0.89</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.28</v>
+        <v>-0.64</v>
       </c>
       <c r="G58" t="n">
-        <v>0.05</v>
+        <v>-0.41</v>
       </c>
     </row>
     <row r="59">
@@ -1797,16 +1797,16 @@
         <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>3.65</v>
+        <v>3.91</v>
       </c>
       <c r="E59" t="n">
-        <v>1.02</v>
+        <v>1.09</v>
       </c>
       <c r="F59" t="n">
-        <v>1.04</v>
+        <v>1.11</v>
       </c>
       <c r="G59" t="n">
-        <v>1.59</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="60">
@@ -1820,16 +1820,16 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>1.63</v>
+        <v>1.36</v>
       </c>
       <c r="E60" t="n">
-        <v>0.68</v>
+        <v>0.51</v>
       </c>
       <c r="F60" t="n">
-        <v>0.53</v>
+        <v>0.45</v>
       </c>
       <c r="G60" t="n">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="61">
@@ -1843,16 +1843,16 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>1.3</v>
+        <v>1.55</v>
       </c>
       <c r="E61" t="n">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="F61" t="n">
-        <v>0.55</v>
+        <v>0.63</v>
       </c>
       <c r="G61" t="n">
-        <v>0.04</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="62">
@@ -1866,16 +1866,16 @@
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.78</v>
+        <v>-0.52</v>
       </c>
       <c r="E62" t="n">
-        <v>0.5</v>
+        <v>0.63</v>
       </c>
       <c r="F62" t="n">
-        <v>0.57</v>
+        <v>0.71</v>
       </c>
       <c r="G62" t="n">
-        <v>-1.85</v>
+        <v>-1.86</v>
       </c>
     </row>
     <row r="63">
@@ -1889,16 +1889,16 @@
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>-2.68</v>
+        <v>-2.2</v>
       </c>
       <c r="E63" t="n">
-        <v>-1.25</v>
+        <v>-1.05</v>
       </c>
       <c r="F63" t="n">
-        <v>-1.29</v>
+        <v>-1.03</v>
       </c>
       <c r="G63" t="n">
-        <v>-0.14</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="64">
@@ -1912,16 +1912,16 @@
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.01</v>
+        <v>-1.4</v>
       </c>
       <c r="E64" t="n">
-        <v>-0.27</v>
+        <v>-0.85</v>
       </c>
       <c r="F64" t="n">
-        <v>-0.25</v>
+        <v>-0.93</v>
       </c>
       <c r="G64" t="n">
-        <v>0.5</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="65">
@@ -1932,19 +1932,19 @@
         <v>11</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>2.64</v>
+        <v>2.94</v>
       </c>
       <c r="E65" t="n">
-        <v>0.94</v>
+        <v>1.05</v>
       </c>
       <c r="F65" t="n">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="G65" t="n">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="66">
@@ -1955,19 +1955,19 @@
         <v>12</v>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="E66" t="n">
-        <v>1.1</v>
+        <v>1.02</v>
       </c>
       <c r="F66" t="n">
-        <v>1.09</v>
+        <v>1.01</v>
       </c>
       <c r="G66" t="n">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="67">
@@ -1981,16 +1981,16 @@
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>-2.12</v>
+        <v>-1.62</v>
       </c>
       <c r="E67" t="n">
-        <v>-1.01</v>
+        <v>-0.8</v>
       </c>
       <c r="F67" t="n">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.11</v>
+        <v>-0.07</v>
       </c>
     </row>
     <row r="68">
@@ -2004,16 +2004,16 @@
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>-4.44</v>
+        <v>-4.39</v>
       </c>
       <c r="E68" t="n">
-        <v>-1.42</v>
+        <v>-1.41</v>
       </c>
       <c r="F68" t="n">
         <v>-1.41</v>
       </c>
       <c r="G68" t="n">
-        <v>-1.6</v>
+        <v>-1.57</v>
       </c>
     </row>
     <row r="69">
@@ -2027,16 +2027,16 @@
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>-1.22</v>
+        <v>-1</v>
       </c>
       <c r="E69" t="n">
-        <v>-0.37</v>
+        <v>-0.27</v>
       </c>
       <c r="F69" t="n">
-        <v>-0.37</v>
+        <v>-0.23</v>
       </c>
       <c r="G69" t="n">
-        <v>-0.48</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="70">
@@ -2050,16 +2050,16 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.94</v>
+        <v>-1.16</v>
       </c>
       <c r="E70" t="n">
-        <v>-0.42</v>
+        <v>-0.5</v>
       </c>
       <c r="F70" t="n">
-        <v>-0.44</v>
+        <v>-0.55</v>
       </c>
       <c r="G70" t="n">
-        <v>-0.08</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="71">
@@ -2073,16 +2073,16 @@
         <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>4.03</v>
+        <v>4.07</v>
       </c>
       <c r="E71" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="F71" t="n">
         <v>1.46</v>
       </c>
-      <c r="F71" t="n">
-        <v>1.45</v>
-      </c>
       <c r="G71" t="n">
-        <v>1.11</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="72">
@@ -2096,16 +2096,16 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="E72" t="n">
-        <v>0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="F72" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>0.07</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="73">
@@ -2119,16 +2119,16 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>2.45</v>
+        <v>2.43</v>
       </c>
       <c r="E73" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F73" t="n">
         <v>0.73</v>
       </c>
-      <c r="F73" t="n">
-        <v>0.75</v>
-      </c>
       <c r="G73" t="n">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="74">
@@ -2142,13 +2142,13 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>-5.32</v>
+        <v>-5.34</v>
       </c>
       <c r="E74" t="n">
-        <v>-1.66</v>
+        <v>-1.68</v>
       </c>
       <c r="F74" t="n">
-        <v>-1.66</v>
+        <v>-1.67</v>
       </c>
       <c r="G74" t="n">
         <v>-1.99</v>
@@ -2165,13 +2165,13 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="E75" t="n">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="F75" t="n">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="G75" t="n">
         <v>0.6</v>
@@ -2188,16 +2188,16 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>2.06</v>
+        <v>2.01</v>
       </c>
       <c r="E76" t="n">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="F76" t="n">
-        <v>1.1</v>
+        <v>1.07</v>
       </c>
       <c r="G76" t="n">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="77">
@@ -2211,16 +2211,16 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.97</v>
+        <v>-0.99</v>
       </c>
       <c r="E77" t="n">
-        <v>-0.69</v>
+        <v>-0.7</v>
       </c>
       <c r="F77" t="n">
         <v>-0.67</v>
       </c>
       <c r="G77" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="78">
@@ -2234,16 +2234,16 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.55</v>
+        <v>0.73</v>
       </c>
       <c r="E78" t="n">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="F78" t="n">
-        <v>0.4</v>
+        <v>0.48</v>
       </c>
       <c r="G78" t="n">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="79">
@@ -2257,13 +2257,13 @@
         <v>1</v>
       </c>
       <c r="D79" t="n">
-        <v>2.21</v>
+        <v>2.16</v>
       </c>
       <c r="E79" t="n">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="F79" t="n">
-        <v>0.6</v>
+        <v>0.57</v>
       </c>
       <c r="G79" t="n">
         <v>0.67</v>
@@ -2280,16 +2280,16 @@
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>-1.82</v>
+        <v>-1.84</v>
       </c>
       <c r="E80" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F80" t="n">
-        <v>-0.16</v>
+        <v>-0.15</v>
       </c>
       <c r="G80" t="n">
-        <v>-1.79</v>
+        <v>-1.81</v>
       </c>
     </row>
     <row r="81">
@@ -2303,16 +2303,16 @@
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>-3.44</v>
+        <v>-3.27</v>
       </c>
       <c r="E81" t="n">
-        <v>-1.93</v>
+        <v>-1.91</v>
       </c>
       <c r="F81" t="n">
-        <v>-1.02</v>
+        <v>-0.93</v>
       </c>
       <c r="G81" t="n">
-        <v>-0.49</v>
+        <v>-0.43</v>
       </c>
     </row>
     <row r="82">
@@ -2326,16 +2326,16 @@
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>-1.35</v>
+        <v>-1.51</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.13</v>
+        <v>-0.17</v>
       </c>
       <c r="F82" t="n">
-        <v>-1.34</v>
+        <v>-1.42</v>
       </c>
       <c r="G82" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="83">
@@ -2349,16 +2349,16 @@
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>2.24</v>
+        <v>2.28</v>
       </c>
       <c r="E83" t="n">
-        <v>0.67</v>
+        <v>0.69</v>
       </c>
       <c r="F83" t="n">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
       <c r="G83" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="84">
@@ -2372,16 +2372,16 @@
         <v>1</v>
       </c>
       <c r="D84" t="n">
-        <v>2.41</v>
+        <v>2.35</v>
       </c>
       <c r="E84" t="n">
         <v>0.72</v>
       </c>
       <c r="F84" t="n">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="G84" t="n">
-        <v>0.77</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="85">
@@ -2395,16 +2395,16 @@
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>1.96</v>
+        <v>1.99</v>
       </c>
       <c r="E85" t="n">
-        <v>0.54</v>
+        <v>0.55</v>
       </c>
       <c r="F85" t="n">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
       <c r="G85" t="n">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="86">
@@ -2441,13 +2441,13 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E87" t="n">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="F87" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
       <c r="G87" t="n">
         <v>-0.04</v>
@@ -2464,16 +2464,16 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>2.31</v>
+        <v>2.22</v>
       </c>
       <c r="E88" t="n">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="F88" t="n">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="G88" t="n">
-        <v>0.8</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="89">
@@ -2487,16 +2487,16 @@
         <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>2.64</v>
+        <v>2.7</v>
       </c>
       <c r="E89" t="n">
-        <v>0.91</v>
+        <v>0.94</v>
       </c>
       <c r="F89" t="n">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="G89" t="n">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="90">
@@ -2513,10 +2513,10 @@
         <v>2.23</v>
       </c>
       <c r="E90" t="n">
-        <v>0.69</v>
+        <v>0.68</v>
       </c>
       <c r="F90" t="n">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="G90" t="n">
         <v>0.73</v>
@@ -2533,10 +2533,10 @@
         <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>-4.23</v>
+        <v>-4.24</v>
       </c>
       <c r="E91" t="n">
-        <v>-1.59</v>
+        <v>-1.6</v>
       </c>
       <c r="F91" t="n">
         <v>-1.52</v>
@@ -2585,7 +2585,7 @@
         <v>-1.34</v>
       </c>
       <c r="F93" t="n">
-        <v>-1.53</v>
+        <v>-1.52</v>
       </c>
       <c r="G93" t="n">
         <v>0.5</v>
@@ -2605,13 +2605,13 @@
         <v>1.92</v>
       </c>
       <c r="E94" t="n">
-        <v>0.8</v>
+        <v>0.79</v>
       </c>
       <c r="F94" t="n">
         <v>0.65</v>
       </c>
       <c r="G94" t="n">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="95">
@@ -2628,7 +2628,7 @@
         <v>1.73</v>
       </c>
       <c r="E95" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="F95" t="n">
         <v>0.65</v>
@@ -2654,7 +2654,7 @@
         <v>0.73</v>
       </c>
       <c r="F96" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="G96" t="n">
         <v>0.26</v>
@@ -2671,13 +2671,13 @@
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>-1.78</v>
+        <v>-1.79</v>
       </c>
       <c r="E97" t="n">
         <v>-1.2</v>
       </c>
       <c r="F97" t="n">
-        <v>-1.01</v>
+        <v>-1.03</v>
       </c>
       <c r="G97" t="n">
         <v>0.44</v>
@@ -2694,16 +2694,16 @@
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>-1.75</v>
+        <v>-1.63</v>
       </c>
       <c r="E98" t="n">
-        <v>0.07</v>
+        <v>0.13</v>
       </c>
       <c r="F98" t="n">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="G98" t="n">
-        <v>-1.99</v>
+        <v>-1.94</v>
       </c>
     </row>
     <row r="99">
@@ -2717,16 +2717,16 @@
         <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>1.05</v>
+        <v>0.99</v>
       </c>
       <c r="E99" t="n">
-        <v>0.49</v>
+        <v>0.51</v>
       </c>
       <c r="F99" t="n">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="G99" t="n">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="100">
@@ -2740,16 +2740,16 @@
         <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>1.18</v>
+        <v>1.26</v>
       </c>
       <c r="E100" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
       <c r="F100" t="n">
         <v>0.37</v>
       </c>
       <c r="G100" t="n">
-        <v>0.54</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="101">
@@ -2763,16 +2763,16 @@
         <v>1</v>
       </c>
       <c r="D101" t="n">
-        <v>2.07</v>
+        <v>2.16</v>
       </c>
       <c r="E101" t="n">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="F101" t="n">
         <v>0.66</v>
       </c>
       <c r="G101" t="n">
-        <v>0.68</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="102">
@@ -2786,16 +2786,16 @@
         <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>1.37</v>
+        <v>1.26</v>
       </c>
       <c r="E102" t="n">
-        <v>0.43</v>
+        <v>0.34</v>
       </c>
       <c r="F102" t="n">
-        <v>0.43</v>
+        <v>0.39</v>
       </c>
       <c r="G102" t="n">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="103">
@@ -2809,16 +2809,16 @@
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>-3.92</v>
+        <v>-4.05</v>
       </c>
       <c r="E103" t="n">
-        <v>-1.99</v>
+        <v>-2</v>
       </c>
       <c r="F103" t="n">
-        <v>-2.01</v>
+        <v>-2.02</v>
       </c>
       <c r="G103" t="n">
-        <v>0.08</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="104">
@@ -2832,16 +2832,16 @@
         <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>-1.75</v>
+        <v>-1.84</v>
       </c>
       <c r="E104" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="F104" t="n">
-        <v>-0.28</v>
+        <v>-0.31</v>
       </c>
       <c r="G104" t="n">
-        <v>-1.7</v>
+        <v>-1.74</v>
       </c>
     </row>
     <row r="105">
@@ -2855,16 +2855,16 @@
         <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>-3.99</v>
+        <v>-3.8</v>
       </c>
       <c r="E105" t="n">
-        <v>-1.98</v>
+        <v>-1.97</v>
       </c>
       <c r="F105" t="n">
-        <v>-1.4</v>
+        <v>-1.29</v>
       </c>
       <c r="G105" t="n">
-        <v>-0.61</v>
+        <v>-0.53</v>
       </c>
     </row>
     <row r="106">
@@ -2878,16 +2878,16 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.43</v>
+        <v>-0.62</v>
       </c>
       <c r="E106" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F106" t="n">
+        <v>-0.77</v>
+      </c>
+      <c r="G106" t="n">
         <v>0.09</v>
-      </c>
-      <c r="F106" t="n">
-        <v>-0.64</v>
-      </c>
-      <c r="G106" t="n">
-        <v>0.11</v>
       </c>
     </row>
     <row r="107">
@@ -2901,16 +2901,16 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>1.24</v>
+        <v>1.29</v>
       </c>
       <c r="E107" t="n">
         <v>0.39</v>
       </c>
       <c r="F107" t="n">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="G107" t="n">
-        <v>0.55</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="108">
@@ -2927,13 +2927,13 @@
         <v>3.27</v>
       </c>
       <c r="E108" t="n">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="F108" t="n">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="G108" t="n">
-        <v>1.01</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="109">
@@ -2947,16 +2947,16 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>1.66</v>
+        <v>1.71</v>
       </c>
       <c r="E109" t="n">
-        <v>0.49</v>
+        <v>0.51</v>
       </c>
       <c r="F109" t="n">
-        <v>0.53</v>
+        <v>0.55</v>
       </c>
       <c r="G109" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="110">
@@ -2970,16 +2970,16 @@
         <v>1</v>
       </c>
       <c r="D110" t="n">
-        <v>2.47</v>
+        <v>2.49</v>
       </c>
       <c r="E110" t="n">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="F110" t="n">
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="G110" t="n">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="111">
@@ -2993,16 +2993,16 @@
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>1.21</v>
+        <v>1.28</v>
       </c>
       <c r="E111" t="n">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
       <c r="F111" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="G111" t="n">
-        <v>0.36</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="112">
@@ -3016,16 +3016,16 @@
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>-2.41</v>
+        <v>-2.63</v>
       </c>
       <c r="E112" t="n">
-        <v>-0.76</v>
+        <v>-0.85</v>
       </c>
       <c r="F112" t="n">
-        <v>-1.35</v>
+        <v>-1.43</v>
       </c>
       <c r="G112" t="n">
-        <v>-0.3</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="113">
@@ -3039,16 +3039,16 @@
         <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>2.36</v>
+        <v>2.4</v>
       </c>
       <c r="E113" t="n">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
       <c r="F113" t="n">
         <v>0.83</v>
       </c>
       <c r="G113" t="n">
-        <v>0.69</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="114">
@@ -3062,16 +3062,16 @@
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>1.08</v>
+        <v>0.99</v>
       </c>
       <c r="E114" t="n">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="F114" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="G114" t="n">
-        <v>0.41</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="115">
@@ -3085,16 +3085,16 @@
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>-4.71</v>
+        <v>-4.53</v>
       </c>
       <c r="E115" t="n">
-        <v>-1.64</v>
+        <v>-1.57</v>
       </c>
       <c r="F115" t="n">
-        <v>-1.18</v>
+        <v>-1.08</v>
       </c>
       <c r="G115" t="n">
-        <v>-1.9</v>
+        <v>-1.87</v>
       </c>
     </row>
     <row r="116">
@@ -3108,16 +3108,16 @@
         <v>0</v>
       </c>
       <c r="D116" t="n">
-        <v>-2.96</v>
+        <v>-0.2</v>
       </c>
       <c r="E116" t="n">
-        <v>-0.18</v>
+        <v>0.26</v>
       </c>
       <c r="F116" t="n">
-        <v>-1.23</v>
+        <v>-0.16</v>
       </c>
       <c r="G116" t="n">
-        <v>-1.55</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="117">
@@ -3128,19 +3128,19 @@
         <v>9</v>
       </c>
       <c r="C117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>1.25</v>
+        <v>-0.14</v>
       </c>
       <c r="E117" t="n">
-        <v>-0.55</v>
+        <v>-0.73</v>
       </c>
       <c r="F117" t="n">
-        <v>1.42</v>
+        <v>0.58</v>
       </c>
       <c r="G117" t="n">
-        <v>0.38</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="118">
@@ -3154,16 +3154,16 @@
         <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>0.97</v>
+        <v>-1.62</v>
       </c>
       <c r="E118" t="n">
-        <v>0.91</v>
+        <v>0.47</v>
       </c>
       <c r="F118" t="n">
-        <v>0.58</v>
+        <v>-0.55</v>
       </c>
       <c r="G118" t="n">
-        <v>-0.52</v>
+        <v>-1.54</v>
       </c>
     </row>
     <row r="119">
@@ -3174,19 +3174,19 @@
         <v>11</v>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D119" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="E119" t="n">
         <v>1.03</v>
       </c>
-      <c r="E119" t="n">
-        <v>0.87</v>
-      </c>
       <c r="F119" t="n">
-        <v>0.51</v>
+        <v>1.44</v>
       </c>
       <c r="G119" t="n">
-        <v>-0.34</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="120">
@@ -3200,16 +3200,16 @@
         <v>0</v>
       </c>
       <c r="D120" t="n">
-        <v>0.82</v>
+        <v>0.59</v>
       </c>
       <c r="E120" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="F120" t="n">
-        <v>-0.79</v>
+        <v>0.2</v>
       </c>
       <c r="G120" t="n">
-        <v>1</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="121">
@@ -3223,16 +3223,16 @@
         <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>-1.12</v>
+        <v>-2.54</v>
       </c>
       <c r="E121" t="n">
         <v>-1.65</v>
       </c>
       <c r="F121" t="n">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="G121" t="n">
-        <v>1.03</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="122">
@@ -3246,10 +3246,10 @@
         <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
       <c r="E122" t="n">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="F122" t="n">
         <v>0.49</v>
@@ -3269,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>-0.49</v>
+        <v>-0.5</v>
       </c>
       <c r="E123" t="n">
-        <v>-1.06</v>
+        <v>-1.07</v>
       </c>
       <c r="F123" t="n">
         <v>0.13</v>
@@ -3292,16 +3292,16 @@
         <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>1.05</v>
+        <v>1.09</v>
       </c>
       <c r="E124" t="n">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="F124" t="n">
         <v>0.45</v>
       </c>
       <c r="G124" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="125">
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>1.75</v>
+        <v>1.73</v>
       </c>
       <c r="E125" t="n">
         <v>0.66</v>
@@ -3324,7 +3324,7 @@
         <v>0.47</v>
       </c>
       <c r="G125" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="126">
@@ -3338,10 +3338,10 @@
         <v>1</v>
       </c>
       <c r="D126" t="n">
-        <v>1.76</v>
+        <v>1.75</v>
       </c>
       <c r="E126" t="n">
-        <v>0.7</v>
+        <v>0.69</v>
       </c>
       <c r="F126" t="n">
         <v>0.48</v>
@@ -3384,16 +3384,16 @@
         <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>-3.32</v>
+        <v>-3.95</v>
       </c>
       <c r="E128" t="n">
-        <v>-1.55</v>
+        <v>-1.87</v>
       </c>
       <c r="F128" t="n">
-        <v>0.14</v>
+        <v>-2</v>
       </c>
       <c r="G128" t="n">
-        <v>-1.91</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="129">
@@ -3407,16 +3407,16 @@
         <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>1.04</v>
+        <v>1.36</v>
       </c>
       <c r="E129" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F129" t="n">
         <v>0.58</v>
       </c>
-      <c r="F129" t="n">
-        <v>0.47</v>
-      </c>
       <c r="G129" t="n">
-        <v>-0.01</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="130">
@@ -3427,19 +3427,19 @@
         <v>10</v>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>1.82</v>
+        <v>2.07</v>
       </c>
       <c r="E130" t="n">
-        <v>0.73</v>
+        <v>0.65</v>
       </c>
       <c r="F130" t="n">
-        <v>0.46</v>
+        <v>0.38</v>
       </c>
       <c r="G130" t="n">
-        <v>0.62</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="131">
@@ -3453,16 +3453,16 @@
         <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>0.88</v>
+        <v>0.32</v>
       </c>
       <c r="E131" t="n">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="F131" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
       <c r="G131" t="n">
-        <v>-0.09</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="132">
@@ -3476,16 +3476,16 @@
         <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>-2.22</v>
+        <v>-2</v>
       </c>
       <c r="E132" t="n">
-        <v>-0.98</v>
+        <v>-0.4</v>
       </c>
       <c r="F132" t="n">
-        <v>-2.02</v>
+        <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>0.78</v>
+        <v>-1.61</v>
       </c>
     </row>
     <row r="133">
@@ -3496,19 +3496,19 @@
         <v>13</v>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>1.8</v>
+        <v>2.21</v>
       </c>
       <c r="E133" t="n">
-        <v>0.71</v>
+        <v>0.63</v>
       </c>
       <c r="F133" t="n">
-        <v>0.48</v>
+        <v>0.55</v>
       </c>
       <c r="G133" t="n">
-        <v>0.6</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="134">
@@ -3522,16 +3522,16 @@
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>-1.56</v>
+        <v>0.91</v>
       </c>
       <c r="E134" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="F134" t="n">
-        <v>-0.03</v>
+        <v>0.05</v>
       </c>
       <c r="G134" t="n">
-        <v>-1.83</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="135">
@@ -3545,16 +3545,16 @@
         <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="E135" t="n">
-        <v>-0.5</v>
+        <v>-0.41</v>
       </c>
       <c r="F135" t="n">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="G135" t="n">
-        <v>0.69</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="136">
@@ -3565,19 +3565,19 @@
         <v>10</v>
       </c>
       <c r="C136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>2.32</v>
+        <v>-1.44</v>
       </c>
       <c r="E136" t="n">
-        <v>0.69</v>
+        <v>0.39</v>
       </c>
       <c r="F136" t="n">
-        <v>0.67</v>
+        <v>0.21</v>
       </c>
       <c r="G136" t="n">
-        <v>0.95</v>
+        <v>-2.04</v>
       </c>
     </row>
     <row r="137">
@@ -3588,19 +3588,19 @@
         <v>11</v>
       </c>
       <c r="C137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137" t="n">
-        <v>0.81</v>
+        <v>1.96</v>
       </c>
       <c r="E137" t="n">
-        <v>0.58</v>
+        <v>0.74</v>
       </c>
       <c r="F137" t="n">
-        <v>0.48</v>
+        <v>0.8</v>
       </c>
       <c r="G137" t="n">
-        <v>-0.24</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="138">
@@ -3614,16 +3614,16 @@
         <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>1.99</v>
+        <v>1.8</v>
       </c>
       <c r="E138" t="n">
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="F138" t="n">
-        <v>0.78</v>
+        <v>0.7</v>
       </c>
       <c r="G138" t="n">
-        <v>0.47</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="139">
@@ -3637,16 +3637,16 @@
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>-3.77</v>
+        <v>-3.39</v>
       </c>
       <c r="E139" t="n">
-        <v>-1.82</v>
+        <v>-1.86</v>
       </c>
       <c r="F139" t="n">
-        <v>-1.92</v>
+        <v>-1.94</v>
       </c>
       <c r="G139" t="n">
-        <v>-0.03</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="140">
@@ -3660,16 +3660,16 @@
         <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>-0.58</v>
+        <v>-1.3</v>
       </c>
       <c r="E140" t="n">
-        <v>0.41</v>
+        <v>0.47</v>
       </c>
       <c r="F140" t="n">
-        <v>0.54</v>
+        <v>0.01</v>
       </c>
       <c r="G140" t="n">
-        <v>-1.53</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="141">
@@ -3683,16 +3683,16 @@
         <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>-4.19</v>
+        <v>-4.07</v>
       </c>
       <c r="E141" t="n">
-        <v>-1.76</v>
+        <v>-1.79</v>
       </c>
       <c r="F141" t="n">
-        <v>-1.84</v>
+        <v>-1.74</v>
       </c>
       <c r="G141" t="n">
-        <v>-0.59</v>
+        <v>-0.54</v>
       </c>
     </row>
     <row r="142">
@@ -3703,19 +3703,19 @@
         <v>10</v>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>1.96</v>
+        <v>1.86</v>
       </c>
       <c r="E142" t="n">
-        <v>0.52</v>
+        <v>0.6</v>
       </c>
       <c r="F142" t="n">
-        <v>0.56</v>
+        <v>0.88</v>
       </c>
       <c r="G142" t="n">
-        <v>0.88</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="143">
@@ -3729,16 +3729,16 @@
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>1.09</v>
+        <v>1.72</v>
       </c>
       <c r="E143" t="n">
-        <v>0.73</v>
+        <v>0.6</v>
       </c>
       <c r="F143" t="n">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="G143" t="n">
-        <v>-0.14</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="144">
@@ -3749,19 +3749,19 @@
         <v>12</v>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>1.62</v>
+        <v>2.15</v>
       </c>
       <c r="E144" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="F144" t="n">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="G144" t="n">
-        <v>0.17</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="145">
@@ -3775,16 +3775,16 @@
         <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>0.1</v>
+        <v>-0.36</v>
       </c>
       <c r="E145" t="n">
-        <v>-0.63</v>
+        <v>-0.6</v>
       </c>
       <c r="F145" t="n">
-        <v>-0.49</v>
+        <v>-0.38</v>
       </c>
       <c r="G145" t="n">
-        <v>1.22</v>
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add report and onset date code
</commit_message>
<xml_diff>
--- a/outcome/appendix/Figure Data/Fig.3 data.xlsx
+++ b/outcome/appendix/Figure Data/Fig.3 data.xlsx
@@ -1,141 +1,158 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stuxmueducn-my.sharepoint.com/personal/kanggle_stu_xmu_edu_cn/Documents/XMU/likangguo/2022/11 COVID_impact_luoli/code_PHSM/outcome/appendix/Figure Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_9AAAD23F0039EB8588A437FA5F3D019852595A2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7259EB3B-00A2-456E-9B0F-08060BC2CA99}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$G$145</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="37">
   <si>
-    <t xml:space="preserve">disease</t>
+    <t>disease</t>
   </si>
   <si>
-    <t xml:space="preserve">Method</t>
+    <t>Method</t>
   </si>
   <si>
-    <t xml:space="preserve">Best</t>
+    <t>Best</t>
   </si>
   <si>
-    <t xml:space="preserve">Index</t>
+    <t>Index</t>
   </si>
   <si>
-    <t xml:space="preserve">norSMAPE</t>
+    <t>norSMAPE</t>
   </si>
   <si>
-    <t xml:space="preserve">norRMSE</t>
+    <t>norRMSE</t>
   </si>
   <si>
-    <t xml:space="preserve">norMASE</t>
+    <t>norMASE</t>
   </si>
   <si>
-    <t xml:space="preserve">HFMD</t>
+    <t>HFMD</t>
   </si>
   <si>
-    <t xml:space="preserve">Neural Network</t>
+    <t>Neural Network</t>
   </si>
   <si>
-    <t xml:space="preserve">Prophet</t>
+    <t>Prophet</t>
   </si>
   <si>
-    <t xml:space="preserve">ETS</t>
+    <t>ETS</t>
   </si>
   <si>
-    <t xml:space="preserve">SARIMA</t>
+    <t>SARIMA</t>
   </si>
   <si>
-    <t xml:space="preserve">Hybrid*</t>
+    <t>Hybrid*</t>
   </si>
   <si>
-    <t xml:space="preserve">Bayesian Structural</t>
+    <t>Bayesian Structural</t>
   </si>
   <si>
-    <t xml:space="preserve">Infectious diarrhea</t>
+    <t>Infectious diarrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">Dysentery</t>
+    <t>Dysentery</t>
   </si>
   <si>
-    <t xml:space="preserve">AHC</t>
+    <t>AHC</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis E</t>
+    <t>Hepatitis E</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A</t>
+    <t>Hepatitis A</t>
   </si>
   <si>
-    <t xml:space="preserve">Enteric fever</t>
+    <t>Enteric fever</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis B</t>
+    <t>Hepatitis B</t>
   </si>
   <si>
-    <t xml:space="preserve">Syphilis</t>
+    <t>Syphilis</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis C</t>
+    <t>Hepatitis C</t>
   </si>
   <si>
-    <t xml:space="preserve">Gonorrhea</t>
+    <t>Gonorrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">AIDS</t>
+    <t>AIDS</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuberculosis</t>
+    <t>Tuberculosis</t>
   </si>
   <si>
-    <t xml:space="preserve">Mumps</t>
+    <t>Mumps</t>
   </si>
   <si>
-    <t xml:space="preserve">Scarlet fever</t>
+    <t>Scarlet fever</t>
   </si>
   <si>
-    <t xml:space="preserve">Rubella</t>
+    <t>Rubella</t>
   </si>
   <si>
-    <t xml:space="preserve">Pertussis</t>
+    <t>Pertussis</t>
   </si>
   <si>
-    <t xml:space="preserve">Brucellosis</t>
+    <t>Brucellosis</t>
   </si>
   <si>
-    <t xml:space="preserve">HFRS</t>
+    <t>HFRS</t>
   </si>
   <si>
-    <t xml:space="preserve">Dengue fever</t>
+    <t>Dengue fever</t>
   </si>
   <si>
-    <t xml:space="preserve">Malaria</t>
+    <t>Malaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Echinococcosis</t>
+    <t>Echinococcosis</t>
   </si>
   <si>
-    <t xml:space="preserve">Typhus</t>
+    <t>Typhus</t>
   </si>
   <si>
-    <t xml:space="preserve">JE</t>
+    <t>JE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -163,9 +180,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -447,14 +473,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,3318 +505,3319 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>-0.2</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F2">
         <v>-0.32</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>0.18</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>-0.11</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>0.22</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.07</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="G3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0.72</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0.49</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>0.16</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>2.37</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>0.64</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>0.71</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>1.02</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="n">
-        <v>2.51</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E6">
         <v>0.77</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>1.03</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>0.71</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>-5.59</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>-1.93</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>-1.8</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>-1.86</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>0.93</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>0.21</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>0.3</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>0.42</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>1.78</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>0.69</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="F9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G9">
         <v>0.52</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>-1.84</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>-0.65</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>-0.53</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>-0.65</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>3.17</v>
       </c>
-      <c r="E11" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="E11">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F11">
         <v>1.04</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>1.02</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>1.08</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>0.3</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>0.39</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>0.4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>-5.12</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>-1.65</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>-1.76</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>-1.71</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>1.42</v>
       </c>
-      <c r="E14" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="E14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F14">
         <v>0.44</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>0.41</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>-0.9</v>
       </c>
-      <c r="E15" t="n">
-        <v>-1.15</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="E15">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="F15">
         <v>0.11</v>
       </c>
-      <c r="G15" t="n">
-        <v>0.14</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="G15">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>1.73</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>0.7</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>0.5</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>0.52</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>1.55</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>0.63</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>0.47</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>0.45</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
         <v>1.66</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>0.67</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>0.49</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>-5.46</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>-1.42</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>-2.02</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>-2.02</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>-0.31</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>0.7</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>0.79</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>-1.8</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>-2.36</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>-1.48</v>
       </c>
-      <c r="F21" t="n">
-        <v>-1.14</v>
-      </c>
-      <c r="G21" t="n">
+      <c r="F21">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="G21">
         <v>0.26</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>0.74</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>0.48</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>0.21</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>0.05</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="E23" t="n">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E23">
         <v>0.66</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>0.77</v>
       </c>
-      <c r="G23" t="n">
-        <v>-0.29</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="G23">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>2.23</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>0.72</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>0.74</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>0.77</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>-1.43</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>-1.07</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>-1.37</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>1.01</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
         <v>-5.56</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>-1.96</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>-1.6</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>-2</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <v>1.66</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>0.46</v>
       </c>
-      <c r="F27" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="G27" t="n">
+      <c r="F27">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G27">
         <v>0.62</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1.16</v>
-      </c>
-      <c r="E28" t="n">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E28">
         <v>0.43</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>0.08</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28">
         <v>0.65</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="n">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>0.67</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>0.24</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29">
         <v>0.12</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G29">
         <v>0.32</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" t="n">
-        <v>2.47</v>
-      </c>
-      <c r="E30" t="n">
+      <c r="D30">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E30">
         <v>0.84</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30">
         <v>1.34</v>
       </c>
-      <c r="G30" t="n">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="G30">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="n">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>-0.4</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31">
         <v>0.01</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F31">
         <v>-0.53</v>
       </c>
-      <c r="G31" t="n">
+      <c r="G31">
         <v>0.12</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>-0.32</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32">
         <v>0.59</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32">
         <v>1.01</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G32">
         <v>-1.91</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>1.72</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33">
         <v>0.19</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F33">
         <v>0.7</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G33">
         <v>0.83</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>1.89</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34">
         <v>0.93</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F34">
         <v>0.6</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34">
         <v>0.35</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>-2.09</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35">
         <v>-0.88</v>
       </c>
-      <c r="F35" t="n">
-        <v>-1.15</v>
-      </c>
-      <c r="G35" t="n">
+      <c r="F35">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="G35">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>0.98</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36">
         <v>0.73</v>
       </c>
-      <c r="F36" t="n">
+      <c r="F36">
         <v>0.17</v>
       </c>
-      <c r="G36" t="n">
-        <v>0.07</v>
-      </c>
-    </row>
-    <row r="37">
+      <c r="G36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>-2.18</v>
-      </c>
-      <c r="E37" t="n">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>-2.1800000000000002</v>
+      </c>
+      <c r="E37">
         <v>-1.56</v>
       </c>
-      <c r="F37" t="n">
+      <c r="F37">
         <v>-1.34</v>
       </c>
-      <c r="G37" t="n">
+      <c r="G37">
         <v>0.72</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>19</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>2.06</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38">
         <v>0.77</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F38">
         <v>0.52</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G38">
         <v>0.78</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
       </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>-0.9</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39">
         <v>-1.5</v>
       </c>
-      <c r="F39" t="n">
+      <c r="F39">
         <v>-0.81</v>
       </c>
-      <c r="G39" t="n">
+      <c r="G39">
         <v>1.41</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
         <v>-0.68</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40">
         <v>0.43</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F40">
         <v>0.37</v>
       </c>
-      <c r="G40" t="n">
+      <c r="G40">
         <v>-1.48</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
         <v>1.49</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E41">
         <v>0.76</v>
       </c>
-      <c r="F41" t="n">
+      <c r="F41">
         <v>0.9</v>
       </c>
-      <c r="G41" t="n">
+      <c r="G41">
         <v>-0.17</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
-      <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="n">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
         <v>0.84</v>
       </c>
-      <c r="E42" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="F42" t="n">
+      <c r="E42">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F42">
         <v>0.66</v>
       </c>
-      <c r="G42" t="n">
+      <c r="G42">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
         <v>-2.81</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E43">
         <v>-1.04</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F43">
         <v>-1.64</v>
       </c>
-      <c r="G43" t="n">
-        <v>-0.14</v>
-      </c>
-    </row>
-    <row r="44">
+      <c r="G43">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>-4.44</v>
-      </c>
-      <c r="E44" t="n">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>-4.4400000000000004</v>
+      </c>
+      <c r="E44">
         <v>-1.8</v>
       </c>
-      <c r="F44" t="n">
+      <c r="F44">
         <v>-1.71</v>
       </c>
-      <c r="G44" t="n">
+      <c r="G44">
         <v>-0.94</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="n">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
         <v>1.2</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45">
         <v>0.4</v>
       </c>
-      <c r="F45" t="n">
+      <c r="F45">
         <v>0.38</v>
       </c>
-      <c r="G45" t="n">
+      <c r="G45">
         <v>0.42</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>2.08</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>0.68</v>
       </c>
-      <c r="F46" t="n">
+      <c r="F46">
         <v>0.63</v>
       </c>
-      <c r="G46" t="n">
+      <c r="G46">
         <v>0.77</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="n">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
         <v>-0.7</v>
       </c>
-      <c r="E47" t="n">
-        <v>-0.28</v>
-      </c>
-      <c r="F47" t="n">
+      <c r="E47">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="F47">
         <v>-0.42</v>
       </c>
-      <c r="G47"/>
-    </row>
-    <row r="48">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
       </c>
-      <c r="C48" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" t="n">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
         <v>-1.29</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>-0.04</v>
       </c>
-      <c r="F48" t="n">
+      <c r="F48">
         <v>-0.06</v>
       </c>
-      <c r="G48" t="n">
+      <c r="G48">
         <v>-1.2</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>3.15</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>1.04</v>
       </c>
-      <c r="F49" t="n">
+      <c r="F49">
         <v>1.17</v>
       </c>
-      <c r="G49" t="n">
+      <c r="G49">
         <v>0.95</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>21</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
-      <c r="C50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" t="n">
-        <v>-4.02</v>
-      </c>
-      <c r="E50" t="n">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>-4.0199999999999996</v>
+      </c>
+      <c r="E50">
         <v>-1.37</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F50">
         <v>-1.41</v>
       </c>
-      <c r="G50" t="n">
+      <c r="G50">
         <v>-1.23</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>21</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
-      <c r="C51" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" t="n">
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
         <v>-3.64</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E51">
         <v>-1.19</v>
       </c>
-      <c r="F51" t="n">
-        <v>-1.14</v>
-      </c>
-      <c r="G51" t="n">
+      <c r="F51">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="G51">
         <v>-1.32</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
-      <c r="C52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" t="n">
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
         <v>1.58</v>
       </c>
-      <c r="E52" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="F52" t="n">
+      <c r="E52">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F52">
         <v>0.5</v>
       </c>
-      <c r="G52" t="n">
+      <c r="G52">
         <v>0.53</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="n">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
         <v>1.84</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E53">
         <v>0.46</v>
       </c>
-      <c r="F53" t="n">
+      <c r="F53">
         <v>0.48</v>
       </c>
-      <c r="G53" t="n">
+      <c r="G53">
         <v>0.9</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>1</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>2.16</v>
       </c>
-      <c r="E54" t="n">
+      <c r="E54">
         <v>0.76</v>
       </c>
-      <c r="F54" t="n">
+      <c r="F54">
         <v>0.77</v>
       </c>
-      <c r="G54" t="n">
+      <c r="G54">
         <v>0.63</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>21</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
       </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
         <v>2.08</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55">
         <v>0.78</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F55">
         <v>0.8</v>
       </c>
-      <c r="G55" t="n">
+      <c r="G55">
         <v>0.5</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>22</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="n">
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
         <v>-3.85</v>
       </c>
-      <c r="E56" t="n">
+      <c r="E56">
         <v>-1.45</v>
       </c>
-      <c r="F56" t="n">
+      <c r="F56">
         <v>-1.66</v>
       </c>
-      <c r="G56" t="n">
+      <c r="G56">
         <v>-0.73</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="n">
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
         <v>-1.07</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57">
         <v>-0.08</v>
       </c>
-      <c r="F57" t="n">
+      <c r="F57">
         <v>0.11</v>
       </c>
-      <c r="G57" t="n">
-        <v>-1.1</v>
-      </c>
-    </row>
-    <row r="58">
+      <c r="G57">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>22</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" t="n">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
         <v>-1.96</v>
       </c>
-      <c r="E58" t="n">
+      <c r="E58">
         <v>-0.9</v>
       </c>
-      <c r="F58" t="n">
+      <c r="F58">
         <v>-0.64</v>
       </c>
-      <c r="G58" t="n">
+      <c r="G58">
         <v>-0.42</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>22</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59">
         <v>1</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59">
         <v>3.85</v>
       </c>
-      <c r="E59" t="n">
+      <c r="E59">
         <v>1.07</v>
       </c>
-      <c r="F59" t="n">
-        <v>1.09</v>
-      </c>
-      <c r="G59" t="n">
+      <c r="F59">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G59">
         <v>1.69</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>22</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C60" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" t="n">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
         <v>1.53</v>
       </c>
-      <c r="E60" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="F60" t="n">
+      <c r="E60">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F60">
         <v>0.5</v>
       </c>
-      <c r="G60" t="n">
+      <c r="G60">
         <v>0.44</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>22</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
       </c>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="n">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
         <v>1.51</v>
       </c>
-      <c r="E61" t="n">
+      <c r="E61">
         <v>0.78</v>
       </c>
-      <c r="F61" t="n">
+      <c r="F61">
         <v>0.61</v>
       </c>
-      <c r="G61" t="n">
+      <c r="G61">
         <v>0.12</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>23</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="n">
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
         <v>-0.5</v>
       </c>
-      <c r="E62" t="n">
+      <c r="E62">
         <v>0.63</v>
       </c>
-      <c r="F62" t="n">
+      <c r="F62">
         <v>0.72</v>
       </c>
-      <c r="G62" t="n">
+      <c r="G62">
         <v>-1.86</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>23</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
-      <c r="C63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" t="n">
-        <v>-2.2</v>
-      </c>
-      <c r="E63" t="n">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="E63">
         <v>-1.05</v>
       </c>
-      <c r="F63" t="n">
+      <c r="F63">
         <v>-1.03</v>
       </c>
-      <c r="G63" t="n">
+      <c r="G63">
         <v>-0.11</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>23</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
       </c>
-      <c r="C64" t="n">
-        <v>0</v>
-      </c>
-      <c r="D64" t="n">
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
         <v>-1.4</v>
       </c>
-      <c r="E64" t="n">
+      <c r="E64">
         <v>-0.85</v>
       </c>
-      <c r="F64" t="n">
+      <c r="F64">
         <v>-0.93</v>
       </c>
-      <c r="G64" t="n">
+      <c r="G64">
         <v>0.37</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>23</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>1</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65">
         <v>2.95</v>
       </c>
-      <c r="E65" t="n">
+      <c r="E65">
         <v>1.06</v>
       </c>
-      <c r="F65" t="n">
+      <c r="F65">
         <v>1</v>
       </c>
-      <c r="G65" t="n">
+      <c r="G65">
         <v>0.9</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
       </c>
-      <c r="C66" t="n">
-        <v>0</v>
-      </c>
-      <c r="D66" t="n">
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
         <v>2.77</v>
       </c>
-      <c r="E66" t="n">
+      <c r="E66">
         <v>1.01</v>
       </c>
-      <c r="F66" t="n">
+      <c r="F66">
         <v>1</v>
       </c>
-      <c r="G66" t="n">
+      <c r="G66">
         <v>0.76</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>23</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
       </c>
-      <c r="C67" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" t="n">
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
         <v>-1.62</v>
       </c>
-      <c r="E67" t="n">
+      <c r="E67">
         <v>-0.8</v>
       </c>
-      <c r="F67" t="n">
+      <c r="F67">
         <v>-0.75</v>
       </c>
-      <c r="G67" t="n">
-        <v>-0.07</v>
-      </c>
-    </row>
-    <row r="68">
+      <c r="G67">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>24</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
       </c>
-      <c r="C68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D68" t="n">
-        <v>-4.36</v>
-      </c>
-      <c r="E68" t="n">
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>-4.3600000000000003</v>
+      </c>
+      <c r="E68">
         <v>-1.4</v>
       </c>
-      <c r="F68" t="n">
+      <c r="F68">
         <v>-1.39</v>
       </c>
-      <c r="G68" t="n">
+      <c r="G68">
         <v>-1.56</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>24</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
-      <c r="C69" t="n">
-        <v>0</v>
-      </c>
-      <c r="D69" t="n">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
         <v>-0.96</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69">
         <v>-0.26</v>
       </c>
-      <c r="F69" t="n">
+      <c r="F69">
         <v>-0.22</v>
       </c>
-      <c r="G69" t="n">
+      <c r="G69">
         <v>-0.48</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>24</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
       </c>
-      <c r="C70" t="n">
-        <v>0</v>
-      </c>
-      <c r="D70" t="n">
-        <v>-1.12</v>
-      </c>
-      <c r="E70" t="n">
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="E70">
         <v>-0.49</v>
       </c>
-      <c r="F70" t="n">
+      <c r="F70">
         <v>-0.53</v>
       </c>
-      <c r="G70" t="n">
+      <c r="G70">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>24</v>
       </c>
       <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="E71" t="n">
+      <c r="D71">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E71">
         <v>1.48</v>
       </c>
-      <c r="F71" t="n">
+      <c r="F71">
         <v>1.47</v>
       </c>
-      <c r="G71" t="n">
-        <v>1.15</v>
-      </c>
-    </row>
-    <row r="72">
+      <c r="G71">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>24</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
       </c>
-      <c r="C72" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" t="n">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
         <v>-0.12</v>
       </c>
-      <c r="E72" t="n">
+      <c r="E72">
         <v>-0.04</v>
       </c>
-      <c r="F72" t="n">
-        <v>-0.07</v>
-      </c>
-      <c r="G72" t="n">
+      <c r="F72">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="G72">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>24</v>
       </c>
       <c r="B73" t="s">
         <v>13</v>
       </c>
-      <c r="C73" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" t="n">
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
         <v>2.46</v>
       </c>
-      <c r="E73" t="n">
+      <c r="E73">
         <v>0.72</v>
       </c>
-      <c r="F73" t="n">
+      <c r="F73">
         <v>0.74</v>
       </c>
-      <c r="G73" t="n">
+      <c r="G73">
         <v>1</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>25</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
       </c>
-      <c r="C74" t="n">
-        <v>0</v>
-      </c>
-      <c r="D74" t="n">
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
         <v>-5.32</v>
       </c>
-      <c r="E74" t="n">
+      <c r="E74">
         <v>-1.67</v>
       </c>
-      <c r="F74" t="n">
+      <c r="F74">
         <v>-1.67</v>
       </c>
-      <c r="G74" t="n">
+      <c r="G74">
         <v>-1.99</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
-      <c r="C75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D75" t="n">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
         <v>1.46</v>
       </c>
-      <c r="E75" t="n">
+      <c r="E75">
         <v>0.62</v>
       </c>
-      <c r="F75" t="n">
+      <c r="F75">
         <v>0.23</v>
       </c>
-      <c r="G75" t="n">
+      <c r="G75">
         <v>0.61</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>25</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
       </c>
-      <c r="C76" t="n">
-        <v>0</v>
-      </c>
-      <c r="D76" t="n">
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
         <v>2.04</v>
       </c>
-      <c r="E76" t="n">
+      <c r="E76">
         <v>0.67</v>
       </c>
-      <c r="F76" t="n">
-        <v>1.09</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0.28</v>
-      </c>
-    </row>
-    <row r="77">
+      <c r="F76">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G76">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>25</v>
       </c>
       <c r="B77" t="s">
         <v>11</v>
       </c>
-      <c r="C77" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" t="n">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
         <v>-0.97</v>
       </c>
-      <c r="E77" t="n">
+      <c r="E77">
         <v>-0.7</v>
       </c>
-      <c r="F77" t="n">
+      <c r="F77">
         <v>-0.67</v>
       </c>
-      <c r="G77" t="n">
+      <c r="G77">
         <v>0.39</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>25</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
       </c>
-      <c r="C78" t="n">
-        <v>0</v>
-      </c>
-      <c r="D78" t="n">
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
         <v>0.6</v>
       </c>
-      <c r="E78" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="F78" t="n">
+      <c r="E78">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F78">
         <v>0.43</v>
       </c>
-      <c r="G78" t="n">
+      <c r="G78">
         <v>0.03</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>25</v>
       </c>
       <c r="B79" t="s">
         <v>13</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79">
         <v>1</v>
       </c>
-      <c r="D79" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E79" t="n">
+      <c r="D79">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E79">
         <v>0.93</v>
       </c>
-      <c r="F79" t="n">
+      <c r="F79">
         <v>0.59</v>
       </c>
-      <c r="G79" t="n">
+      <c r="G79">
         <v>0.68</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>26</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
       </c>
-      <c r="C80" t="n">
-        <v>0</v>
-      </c>
-      <c r="D80" t="n">
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
         <v>-1.85</v>
       </c>
-      <c r="E80" t="n">
+      <c r="E80">
         <v>0.12</v>
       </c>
-      <c r="F80" t="n">
+      <c r="F80">
         <v>-0.16</v>
       </c>
-      <c r="G80" t="n">
+      <c r="G80">
         <v>-1.81</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>26</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
-      <c r="C81" t="n">
-        <v>0</v>
-      </c>
-      <c r="D81" t="n">
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
         <v>-3.27</v>
       </c>
-      <c r="E81" t="n">
+      <c r="E81">
         <v>-1.91</v>
       </c>
-      <c r="F81" t="n">
+      <c r="F81">
         <v>-0.93</v>
       </c>
-      <c r="G81" t="n">
+      <c r="G81">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
       </c>
-      <c r="C82" t="n">
-        <v>0</v>
-      </c>
-      <c r="D82" t="n">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
         <v>-1.51</v>
       </c>
-      <c r="E82" t="n">
+      <c r="E82">
         <v>-0.18</v>
       </c>
-      <c r="F82" t="n">
+      <c r="F82">
         <v>-1.42</v>
       </c>
-      <c r="G82" t="n">
+      <c r="G82">
         <v>0.08</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>26</v>
       </c>
       <c r="B83" t="s">
         <v>11</v>
       </c>
-      <c r="C83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D83" t="n">
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
         <v>2.27</v>
       </c>
-      <c r="E83" t="n">
+      <c r="E83">
         <v>0.69</v>
       </c>
-      <c r="F83" t="n">
+      <c r="F83">
         <v>0.87</v>
       </c>
-      <c r="G83" t="n">
+      <c r="G83">
         <v>0.72</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>26</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84">
         <v>1</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84">
         <v>2.37</v>
       </c>
-      <c r="E84" t="n">
+      <c r="E84">
         <v>0.73</v>
       </c>
-      <c r="F84" t="n">
+      <c r="F84">
         <v>0.89</v>
       </c>
-      <c r="G84" t="n">
+      <c r="G84">
         <v>0.75</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>26</v>
       </c>
       <c r="B85" t="s">
         <v>13</v>
       </c>
-      <c r="C85" t="n">
-        <v>0</v>
-      </c>
-      <c r="D85" t="n">
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
         <v>1.98</v>
       </c>
-      <c r="E85" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="F85" t="n">
+      <c r="E85">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F85">
         <v>0.75</v>
       </c>
-      <c r="G85" t="n">
+      <c r="G85">
         <v>0.69</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>27</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
       </c>
-      <c r="C86" t="n">
-        <v>0</v>
-      </c>
-      <c r="D86" t="n">
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
         <v>-2.97</v>
       </c>
-      <c r="E86" t="n">
+      <c r="E86">
         <v>-0.76</v>
       </c>
-      <c r="F86" t="n">
+      <c r="F86">
         <v>-0.91</v>
       </c>
-      <c r="G86" t="n">
+      <c r="G86">
         <v>-1.3</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>27</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
-      <c r="C87" t="n">
-        <v>0</v>
-      </c>
-      <c r="D87" t="n">
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
         <v>0.05</v>
       </c>
-      <c r="E87" t="n">
+      <c r="E87">
         <v>0.01</v>
       </c>
-      <c r="F87" t="n">
+      <c r="F87">
         <v>0.08</v>
       </c>
-      <c r="G87" t="n">
+      <c r="G87">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>27</v>
       </c>
       <c r="B88" t="s">
         <v>10</v>
       </c>
-      <c r="C88" t="n">
-        <v>0</v>
-      </c>
-      <c r="D88" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="E88" t="n">
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="E88">
         <v>0.72</v>
       </c>
-      <c r="F88" t="n">
+      <c r="F88">
         <v>0.71</v>
       </c>
-      <c r="G88" t="n">
+      <c r="G88">
         <v>0.79</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>27</v>
       </c>
       <c r="B89" t="s">
         <v>11</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89">
         <v>1</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89">
         <v>2.7</v>
       </c>
-      <c r="E89" t="n">
+      <c r="E89">
         <v>0.94</v>
       </c>
-      <c r="F89" t="n">
+      <c r="F89">
         <v>0.82</v>
       </c>
-      <c r="G89" t="n">
+      <c r="G89">
         <v>0.94</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>27</v>
       </c>
       <c r="B90" t="s">
         <v>12</v>
       </c>
-      <c r="C90" t="n">
-        <v>0</v>
-      </c>
-      <c r="D90" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="E90" t="n">
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E90">
         <v>0.69</v>
       </c>
-      <c r="F90" t="n">
+      <c r="F90">
         <v>0.82</v>
       </c>
-      <c r="G90" t="n">
+      <c r="G90">
         <v>0.73</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>27</v>
       </c>
       <c r="B91" t="s">
         <v>13</v>
       </c>
-      <c r="C91" t="n">
-        <v>0</v>
-      </c>
-      <c r="D91" t="n">
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
         <v>-4.24</v>
       </c>
-      <c r="E91" t="n">
+      <c r="E91">
         <v>-1.6</v>
       </c>
-      <c r="F91" t="n">
+      <c r="F91">
         <v>-1.52</v>
       </c>
-      <c r="G91" t="n">
-        <v>-1.12</v>
-      </c>
-    </row>
-    <row r="92">
+      <c r="G91">
+        <v>-1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>28</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
       </c>
-      <c r="C92" t="n">
-        <v>0</v>
-      </c>
-      <c r="D92" t="n">
-        <v>-1.13</v>
-      </c>
-      <c r="E92" t="n">
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="E92">
         <v>0.3</v>
       </c>
-      <c r="F92" t="n">
+      <c r="F92">
         <v>0.6</v>
       </c>
-      <c r="G92" t="n">
-        <v>-2.03</v>
-      </c>
-    </row>
-    <row r="93">
+      <c r="G92">
+        <v>-2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>28</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
-      <c r="C93" t="n">
-        <v>0</v>
-      </c>
-      <c r="D93" t="n">
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
         <v>-2.37</v>
       </c>
-      <c r="E93" t="n">
+      <c r="E93">
         <v>-1.34</v>
       </c>
-      <c r="F93" t="n">
+      <c r="F93">
         <v>-1.52</v>
       </c>
-      <c r="G93" t="n">
+      <c r="G93">
         <v>0.5</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>28</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94">
         <v>1</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94">
         <v>1.92</v>
       </c>
-      <c r="E94" t="n">
+      <c r="E94">
         <v>0.79</v>
       </c>
-      <c r="F94" t="n">
+      <c r="F94">
         <v>0.65</v>
       </c>
-      <c r="G94" t="n">
+      <c r="G94">
         <v>0.47</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
       <c r="B95" t="s">
         <v>11</v>
       </c>
-      <c r="C95" t="n">
-        <v>0</v>
-      </c>
-      <c r="D95" t="n">
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
         <v>1.73</v>
       </c>
-      <c r="E95" t="n">
+      <c r="E95">
         <v>0.72</v>
       </c>
-      <c r="F95" t="n">
+      <c r="F95">
         <v>0.65</v>
       </c>
-      <c r="G95" t="n">
+      <c r="G95">
         <v>0.37</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>28</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
-      <c r="C96" t="n">
-        <v>0</v>
-      </c>
-      <c r="D96" t="n">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
         <v>1.63</v>
       </c>
-      <c r="E96" t="n">
+      <c r="E96">
         <v>0.73</v>
       </c>
-      <c r="F96" t="n">
+      <c r="F96">
         <v>0.65</v>
       </c>
-      <c r="G96" t="n">
+      <c r="G96">
         <v>0.26</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>28</v>
       </c>
       <c r="B97" t="s">
         <v>13</v>
       </c>
-      <c r="C97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D97" t="n">
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
         <v>-1.79</v>
       </c>
-      <c r="E97" t="n">
+      <c r="E97">
         <v>-1.2</v>
       </c>
-      <c r="F97" t="n">
+      <c r="F97">
         <v>-1.03</v>
       </c>
-      <c r="G97" t="n">
+      <c r="G97">
         <v>0.44</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>29</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
       </c>
-      <c r="C98" t="n">
-        <v>0</v>
-      </c>
-      <c r="D98" t="n">
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
         <v>-1.65</v>
       </c>
-      <c r="E98" t="n">
+      <c r="E98">
         <v>0.11</v>
       </c>
-      <c r="F98" t="n">
+      <c r="F98">
         <v>0.18</v>
       </c>
-      <c r="G98" t="n">
+      <c r="G98">
         <v>-1.94</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>29</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
-      <c r="C99" t="n">
-        <v>0</v>
-      </c>
-      <c r="D99" t="n">
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
         <v>0.96</v>
       </c>
-      <c r="E99" t="n">
+      <c r="E99">
         <v>0.49</v>
       </c>
-      <c r="F99" t="n">
+      <c r="F99">
         <v>0.4</v>
       </c>
-      <c r="G99" t="n">
-        <v>0.07</v>
-      </c>
-    </row>
-    <row r="100">
+      <c r="G99">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>29</v>
       </c>
       <c r="B100" t="s">
         <v>10</v>
       </c>
-      <c r="C100" t="n">
-        <v>0</v>
-      </c>
-      <c r="D100" t="n">
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
         <v>1.23</v>
       </c>
-      <c r="E100" t="n">
+      <c r="E100">
         <v>0.27</v>
       </c>
-      <c r="F100" t="n">
+      <c r="F100">
         <v>0.37</v>
       </c>
-      <c r="G100" t="n">
+      <c r="G100">
         <v>0.6</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>29</v>
       </c>
       <c r="B101" t="s">
         <v>11</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101">
         <v>1</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101">
         <v>2.13</v>
       </c>
-      <c r="E101" t="n">
+      <c r="E101">
         <v>0.72</v>
       </c>
-      <c r="F101" t="n">
+      <c r="F101">
         <v>0.66</v>
       </c>
-      <c r="G101" t="n">
+      <c r="G101">
         <v>0.76</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>29</v>
       </c>
       <c r="B102" t="s">
         <v>12</v>
       </c>
-      <c r="C102" t="n">
-        <v>0</v>
-      </c>
-      <c r="D102" t="n">
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
         <v>1.37</v>
       </c>
-      <c r="E102" t="n">
+      <c r="E102">
         <v>0.41</v>
       </c>
-      <c r="F102" t="n">
+      <c r="F102">
         <v>0.42</v>
       </c>
-      <c r="G102" t="n">
+      <c r="G102">
         <v>0.54</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>29</v>
       </c>
       <c r="B103" t="s">
         <v>13</v>
       </c>
-      <c r="C103" t="n">
-        <v>0</v>
-      </c>
-      <c r="D103" t="n">
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
         <v>-4.05</v>
       </c>
-      <c r="E103" t="n">
+      <c r="E103">
         <v>-2</v>
       </c>
-      <c r="F103" t="n">
+      <c r="F103">
         <v>-2.02</v>
       </c>
-      <c r="G103" t="n">
+      <c r="G103">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>30</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
       </c>
-      <c r="C104" t="n">
-        <v>0</v>
-      </c>
-      <c r="D104" t="n">
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
         <v>-1.84</v>
       </c>
-      <c r="E104" t="n">
+      <c r="E104">
         <v>0.21</v>
       </c>
-      <c r="F104" t="n">
+      <c r="F104">
         <v>-0.31</v>
       </c>
-      <c r="G104" t="n">
+      <c r="G104">
         <v>-1.74</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>30</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
-      <c r="C105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D105" t="n">
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
         <v>-3.8</v>
       </c>
-      <c r="E105" t="n">
+      <c r="E105">
         <v>-1.97</v>
       </c>
-      <c r="F105" t="n">
+      <c r="F105">
         <v>-1.29</v>
       </c>
-      <c r="G105" t="n">
+      <c r="G105">
         <v>-0.54</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>30</v>
       </c>
       <c r="B106" t="s">
         <v>10</v>
       </c>
-      <c r="C106" t="n">
-        <v>0</v>
-      </c>
-      <c r="D106" t="n">
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
         <v>-0.62</v>
       </c>
-      <c r="E106" t="n">
+      <c r="E106">
         <v>0.06</v>
       </c>
-      <c r="F106" t="n">
+      <c r="F106">
         <v>-0.77</v>
       </c>
-      <c r="G106" t="n">
+      <c r="G106">
         <v>0.09</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>30</v>
       </c>
       <c r="B107" t="s">
         <v>11</v>
       </c>
-      <c r="C107" t="n">
-        <v>0</v>
-      </c>
-      <c r="D107" t="n">
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
         <v>1.28</v>
       </c>
-      <c r="E107" t="n">
+      <c r="E107">
         <v>0.39</v>
       </c>
-      <c r="F107" t="n">
+      <c r="F107">
         <v>0.33</v>
       </c>
-      <c r="G107" t="n">
-        <v>0.56</v>
-      </c>
-    </row>
-    <row r="108">
+      <c r="G107">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>30</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108">
         <v>1</v>
       </c>
-      <c r="D108" t="n">
+      <c r="D108">
         <v>3.29</v>
       </c>
-      <c r="E108" t="n">
+      <c r="E108">
         <v>0.81</v>
       </c>
-      <c r="F108" t="n">
+      <c r="F108">
         <v>1.5</v>
       </c>
-      <c r="G108" t="n">
+      <c r="G108">
         <v>0.98</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>30</v>
       </c>
       <c r="B109" t="s">
         <v>13</v>
       </c>
-      <c r="C109" t="n">
-        <v>0</v>
-      </c>
-      <c r="D109" t="n">
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
         <v>1.69</v>
       </c>
-      <c r="E109" t="n">
+      <c r="E109">
         <v>0.5</v>
       </c>
-      <c r="F109" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="G109" t="n">
+      <c r="F109">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G109">
         <v>0.64</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>31</v>
       </c>
       <c r="B110" t="s">
         <v>8</v>
       </c>
-      <c r="C110" t="n">
+      <c r="C110">
         <v>1</v>
       </c>
-      <c r="D110" t="n">
-        <v>2.47</v>
-      </c>
-      <c r="E110" t="n">
+      <c r="D110">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E110">
         <v>0.92</v>
       </c>
-      <c r="F110" t="n">
+      <c r="F110">
         <v>0.8</v>
       </c>
-      <c r="G110" t="n">
+      <c r="G110">
         <v>0.75</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>31</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
       </c>
-      <c r="C111" t="n">
-        <v>0</v>
-      </c>
-      <c r="D111" t="n">
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
         <v>1.26</v>
       </c>
-      <c r="E111" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="F111" t="n">
+      <c r="E111">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F111">
         <v>0.61</v>
       </c>
-      <c r="G111" t="n">
+      <c r="G111">
         <v>0.38</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>31</v>
       </c>
       <c r="B112" t="s">
         <v>10</v>
       </c>
-      <c r="C112" t="n">
-        <v>0</v>
-      </c>
-      <c r="D112" t="n">
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
         <v>-2.64</v>
       </c>
-      <c r="E112" t="n">
+      <c r="E112">
         <v>-0.86</v>
       </c>
-      <c r="F112" t="n">
+      <c r="F112">
         <v>-1.43</v>
       </c>
-      <c r="G112" t="n">
+      <c r="G112">
         <v>-0.35</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>31</v>
       </c>
       <c r="B113" t="s">
         <v>11</v>
       </c>
-      <c r="C113" t="n">
-        <v>0</v>
-      </c>
-      <c r="D113" t="n">
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
         <v>2.38</v>
       </c>
-      <c r="E113" t="n">
+      <c r="E113">
         <v>0.86</v>
       </c>
-      <c r="F113" t="n">
+      <c r="F113">
         <v>0.82</v>
       </c>
-      <c r="G113" t="n">
+      <c r="G113">
         <v>0.71</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>31</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
       </c>
-      <c r="C114" t="n">
-        <v>0</v>
-      </c>
-      <c r="D114" t="n">
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
         <v>1.06</v>
       </c>
-      <c r="E114" t="n">
+      <c r="E114">
         <v>0.37</v>
       </c>
-      <c r="F114" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="G114" t="n">
+      <c r="F114">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G114">
         <v>0.39</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>31</v>
       </c>
       <c r="B115" t="s">
         <v>13</v>
       </c>
-      <c r="C115" t="n">
-        <v>0</v>
-      </c>
-      <c r="D115" t="n">
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
         <v>-4.53</v>
       </c>
-      <c r="E115" t="n">
+      <c r="E115">
         <v>-1.57</v>
       </c>
-      <c r="F115" t="n">
+      <c r="F115">
         <v>-1.08</v>
       </c>
-      <c r="G115" t="n">
+      <c r="G115">
         <v>-1.88</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>32</v>
       </c>
       <c r="B116" t="s">
         <v>8</v>
       </c>
-      <c r="C116" t="n">
-        <v>0</v>
-      </c>
-      <c r="D116" t="n">
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
         <v>-0.24</v>
       </c>
-      <c r="E116" t="n">
+      <c r="E116">
         <v>0.26</v>
       </c>
-      <c r="F116" t="n">
+      <c r="F116">
         <v>-0.17</v>
       </c>
-      <c r="G116" t="n">
+      <c r="G116">
         <v>-0.34</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>32</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
       </c>
-      <c r="C117" t="n">
-        <v>0</v>
-      </c>
-      <c r="D117" t="n">
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
         <v>-0.18</v>
       </c>
-      <c r="E117" t="n">
+      <c r="E117">
         <v>-0.73</v>
       </c>
-      <c r="F117" t="n">
-        <v>0.56</v>
-      </c>
-      <c r="G117" t="n">
+      <c r="F117">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G117">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>32</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
       </c>
-      <c r="C118" t="n">
-        <v>0</v>
-      </c>
-      <c r="D118" t="n">
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
         <v>-1.66</v>
       </c>
-      <c r="E118" t="n">
+      <c r="E118">
         <v>0.48</v>
       </c>
-      <c r="F118" t="n">
-        <v>-0.56</v>
-      </c>
-      <c r="G118" t="n">
+      <c r="F118">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="G118">
         <v>-1.58</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>32</v>
       </c>
       <c r="B119" t="s">
         <v>11</v>
       </c>
-      <c r="C119" t="n">
+      <c r="C119">
         <v>1</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D119">
         <v>3.88</v>
       </c>
-      <c r="E119" t="n">
+      <c r="E119">
         <v>1.03</v>
       </c>
-      <c r="F119" t="n">
+      <c r="F119">
         <v>1.42</v>
       </c>
-      <c r="G119" t="n">
+      <c r="G119">
         <v>1.43</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>32</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
       </c>
-      <c r="C120" t="n">
-        <v>0</v>
-      </c>
-      <c r="D120" t="n">
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
         <v>0.78</v>
       </c>
-      <c r="E120" t="n">
+      <c r="E120">
         <v>0.61</v>
       </c>
-      <c r="F120" t="n">
+      <c r="F120">
         <v>0.25</v>
       </c>
-      <c r="G120" t="n">
+      <c r="G120">
         <v>-0.09</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>32</v>
       </c>
       <c r="B121" t="s">
         <v>13</v>
       </c>
-      <c r="C121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D121" t="n">
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
         <v>-2.57</v>
       </c>
-      <c r="E121" t="n">
+      <c r="E121">
         <v>-1.65</v>
       </c>
-      <c r="F121" t="n">
+      <c r="F121">
         <v>-1.5</v>
       </c>
-      <c r="G121" t="n">
-        <v>0.58</v>
-      </c>
-    </row>
-    <row r="122">
+      <c r="G121">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>33</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
       </c>
-      <c r="C122" t="n">
-        <v>0</v>
-      </c>
-      <c r="D122" t="n">
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
         <v>1.44</v>
       </c>
-      <c r="E122" t="n">
+      <c r="E122">
         <v>0.73</v>
       </c>
-      <c r="F122" t="n">
+      <c r="F122">
         <v>0.49</v>
       </c>
-      <c r="G122" t="n">
+      <c r="G122">
         <v>0.23</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>33</v>
       </c>
       <c r="B123" t="s">
         <v>9</v>
       </c>
-      <c r="C123" t="n">
-        <v>0</v>
-      </c>
-      <c r="D123" t="n">
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
         <v>-0.5</v>
       </c>
-      <c r="E123" t="n">
+      <c r="E123">
         <v>-1.07</v>
       </c>
-      <c r="F123" t="n">
+      <c r="F123">
         <v>0.13</v>
       </c>
-      <c r="G123" t="n">
+      <c r="G123">
         <v>0.44</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>33</v>
       </c>
       <c r="B124" t="s">
         <v>10</v>
       </c>
-      <c r="C124" t="n">
-        <v>0</v>
-      </c>
-      <c r="D124" t="n">
-        <v>1.09</v>
-      </c>
-      <c r="E124" t="n">
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E124">
         <v>0.47</v>
       </c>
-      <c r="F124" t="n">
+      <c r="F124">
         <v>0.45</v>
       </c>
-      <c r="G124" t="n">
+      <c r="G124">
         <v>0.16</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>33</v>
       </c>
       <c r="B125" t="s">
         <v>11</v>
       </c>
-      <c r="C125" t="n">
-        <v>0</v>
-      </c>
-      <c r="D125" t="n">
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
         <v>1.73</v>
       </c>
-      <c r="E125" t="n">
+      <c r="E125">
         <v>0.66</v>
       </c>
-      <c r="F125" t="n">
+      <c r="F125">
         <v>0.47</v>
       </c>
-      <c r="G125" t="n">
+      <c r="G125">
         <v>0.6</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>33</v>
       </c>
       <c r="B126" t="s">
         <v>12</v>
       </c>
-      <c r="C126" t="n">
+      <c r="C126">
         <v>1</v>
       </c>
-      <c r="D126" t="n">
+      <c r="D126">
         <v>1.75</v>
       </c>
-      <c r="E126" t="n">
+      <c r="E126">
         <v>0.69</v>
       </c>
-      <c r="F126" t="n">
+      <c r="F126">
         <v>0.48</v>
       </c>
-      <c r="G126" t="n">
-        <v>0.58</v>
-      </c>
-    </row>
-    <row r="127">
+      <c r="G126">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>33</v>
       </c>
       <c r="B127" t="s">
         <v>13</v>
       </c>
-      <c r="C127" t="n">
-        <v>0</v>
-      </c>
-      <c r="D127" t="n">
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
         <v>-5.51</v>
       </c>
-      <c r="E127" t="n">
+      <c r="E127">
         <v>-1.48</v>
       </c>
-      <c r="F127" t="n">
+      <c r="F127">
         <v>-2.02</v>
       </c>
-      <c r="G127" t="n">
-        <v>-2.01</v>
-      </c>
-    </row>
-    <row r="128">
+      <c r="G127">
+        <v>-2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>34</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
       </c>
-      <c r="C128" t="n">
-        <v>0</v>
-      </c>
-      <c r="D128" t="n">
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
         <v>-3.91</v>
       </c>
-      <c r="E128" t="n">
+      <c r="E128">
         <v>-1.85</v>
       </c>
-      <c r="F128" t="n">
+      <c r="F128">
         <v>-1.98</v>
       </c>
-      <c r="G128" t="n">
+      <c r="G128">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>34</v>
       </c>
       <c r="B129" t="s">
         <v>9</v>
       </c>
-      <c r="C129" t="n">
-        <v>0</v>
-      </c>
-      <c r="D129" t="n">
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
         <v>1.38</v>
       </c>
-      <c r="E129" t="n">
+      <c r="E129">
         <v>0.66</v>
       </c>
-      <c r="F129" t="n">
+      <c r="F129">
         <v>0.59</v>
       </c>
-      <c r="G129" t="n">
+      <c r="G129">
         <v>0.12</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>34</v>
       </c>
       <c r="B130" t="s">
         <v>10</v>
       </c>
-      <c r="C130" t="n">
-        <v>0</v>
-      </c>
-      <c r="D130" t="n">
-        <v>2.07</v>
-      </c>
-      <c r="E130" t="n">
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E130">
         <v>0.66</v>
       </c>
-      <c r="F130" t="n">
+      <c r="F130">
         <v>0.39</v>
       </c>
-      <c r="G130" t="n">
+      <c r="G130">
         <v>1.03</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>34</v>
       </c>
       <c r="B131" t="s">
         <v>11</v>
       </c>
-      <c r="C131" t="n">
-        <v>0</v>
-      </c>
-      <c r="D131" t="n">
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
         <v>0.36</v>
       </c>
-      <c r="E131" t="n">
+      <c r="E131">
         <v>0.34</v>
       </c>
-      <c r="F131" t="n">
+      <c r="F131">
         <v>0.5</v>
       </c>
-      <c r="G131" t="n">
+      <c r="G131">
         <v>-0.48</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>34</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
       </c>
-      <c r="C132" t="n">
-        <v>0</v>
-      </c>
-      <c r="D132" t="n">
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
         <v>-2.12</v>
       </c>
-      <c r="E132" t="n">
+      <c r="E132">
         <v>-0.44</v>
       </c>
-      <c r="F132" t="n">
+      <c r="F132">
         <v>-0.05</v>
       </c>
-      <c r="G132" t="n">
+      <c r="G132">
         <v>-1.62</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>34</v>
       </c>
       <c r="B133" t="s">
         <v>13</v>
       </c>
-      <c r="C133" t="n">
+      <c r="C133">
         <v>1</v>
       </c>
-      <c r="D133" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="E133" t="n">
+      <c r="D133">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="E133">
         <v>0.63</v>
       </c>
-      <c r="F133" t="n">
-        <v>0.56</v>
-      </c>
-      <c r="G133" t="n">
+      <c r="F133">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G133">
         <v>1.02</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>35</v>
       </c>
       <c r="B134" t="s">
         <v>8</v>
       </c>
-      <c r="C134" t="n">
-        <v>0</v>
-      </c>
-      <c r="D134" t="n">
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
         <v>0.91</v>
       </c>
-      <c r="E134" t="n">
+      <c r="E134">
         <v>0.45</v>
       </c>
-      <c r="F134" t="n">
+      <c r="F134">
         <v>0.05</v>
       </c>
-      <c r="G134" t="n">
+      <c r="G134">
         <v>0.41</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>35</v>
       </c>
       <c r="B135" t="s">
         <v>9</v>
       </c>
-      <c r="C135" t="n">
-        <v>0</v>
-      </c>
-      <c r="D135" t="n">
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
         <v>0.18</v>
       </c>
-      <c r="E135" t="n">
+      <c r="E135">
         <v>-0.41</v>
       </c>
-      <c r="F135" t="n">
+      <c r="F135">
         <v>0.18</v>
       </c>
-      <c r="G135" t="n">
+      <c r="G135">
         <v>0.41</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>35</v>
       </c>
       <c r="B136" t="s">
         <v>10</v>
       </c>
-      <c r="C136" t="n">
-        <v>0</v>
-      </c>
-      <c r="D136" t="n">
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
         <v>-1.43</v>
       </c>
-      <c r="E136" t="n">
+      <c r="E136">
         <v>0.39</v>
       </c>
-      <c r="F136" t="n">
+      <c r="F136">
         <v>0.22</v>
       </c>
-      <c r="G136" t="n">
+      <c r="G136">
         <v>-2.04</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>35</v>
       </c>
       <c r="B137" t="s">
         <v>11</v>
       </c>
-      <c r="C137" t="n">
+      <c r="C137">
         <v>1</v>
       </c>
-      <c r="D137" t="n">
+      <c r="D137">
         <v>1.96</v>
       </c>
-      <c r="E137" t="n">
+      <c r="E137">
         <v>0.74</v>
       </c>
-      <c r="F137" t="n">
+      <c r="F137">
         <v>0.81</v>
       </c>
-      <c r="G137" t="n">
+      <c r="G137">
         <v>0.41</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>35</v>
       </c>
       <c r="B138" t="s">
         <v>12</v>
       </c>
-      <c r="C138" t="n">
-        <v>0</v>
-      </c>
-      <c r="D138" t="n">
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
         <v>1.78</v>
       </c>
-      <c r="E138" t="n">
+      <c r="E138">
         <v>0.69</v>
       </c>
-      <c r="F138" t="n">
+      <c r="F138">
         <v>0.69</v>
       </c>
-      <c r="G138" t="n">
+      <c r="G138">
         <v>0.41</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>35</v>
       </c>
       <c r="B139" t="s">
         <v>13</v>
       </c>
-      <c r="C139" t="n">
-        <v>0</v>
-      </c>
-      <c r="D139" t="n">
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
         <v>-3.4</v>
       </c>
-      <c r="E139" t="n">
+      <c r="E139">
         <v>-1.86</v>
       </c>
-      <c r="F139" t="n">
+      <c r="F139">
         <v>-1.95</v>
       </c>
-      <c r="G139" t="n">
+      <c r="G139">
         <v>0.41</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>36</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
       </c>
-      <c r="C140" t="n">
-        <v>0</v>
-      </c>
-      <c r="D140" t="n">
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
         <v>-1.3</v>
       </c>
-      <c r="E140" t="n">
+      <c r="E140">
         <v>0.47</v>
       </c>
-      <c r="F140" t="n">
+      <c r="F140">
         <v>0.01</v>
       </c>
-      <c r="G140" t="n">
+      <c r="G140">
         <v>-1.79</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>36</v>
       </c>
       <c r="B141" t="s">
         <v>9</v>
       </c>
-      <c r="C141" t="n">
-        <v>0</v>
-      </c>
-      <c r="D141" t="n">
-        <v>-4.06</v>
-      </c>
-      <c r="E141" t="n">
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>-4.0599999999999996</v>
+      </c>
+      <c r="E141">
         <v>-1.79</v>
       </c>
-      <c r="F141" t="n">
+      <c r="F141">
         <v>-1.74</v>
       </c>
-      <c r="G141" t="n">
+      <c r="G141">
         <v>-0.54</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>36</v>
       </c>
       <c r="B142" t="s">
         <v>10</v>
       </c>
-      <c r="C142" t="n">
-        <v>0</v>
-      </c>
-      <c r="D142" t="n">
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
         <v>1.86</v>
       </c>
-      <c r="E142" t="n">
+      <c r="E142">
         <v>0.6</v>
       </c>
-      <c r="F142" t="n">
+      <c r="F142">
         <v>0.88</v>
       </c>
-      <c r="G142" t="n">
+      <c r="G142">
         <v>0.38</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>36</v>
       </c>
       <c r="B143" t="s">
         <v>11</v>
       </c>
-      <c r="C143" t="n">
-        <v>0</v>
-      </c>
-      <c r="D143" t="n">
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
         <v>1.72</v>
       </c>
-      <c r="E143" t="n">
+      <c r="E143">
         <v>0.6</v>
       </c>
-      <c r="F143" t="n">
+      <c r="F143">
         <v>0.22</v>
       </c>
-      <c r="G143" t="n">
+      <c r="G143">
         <v>0.91</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>36</v>
       </c>
       <c r="B144" t="s">
         <v>12</v>
       </c>
-      <c r="C144" t="n">
+      <c r="C144">
         <v>1</v>
       </c>
-      <c r="D144" t="n">
+      <c r="D144">
         <v>2.15</v>
       </c>
-      <c r="E144" t="n">
+      <c r="E144">
         <v>0.72</v>
       </c>
-      <c r="F144" t="n">
+      <c r="F144">
         <v>1.01</v>
       </c>
-      <c r="G144" t="n">
+      <c r="G144">
         <v>0.42</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>36</v>
       </c>
       <c r="B145" t="s">
         <v>13</v>
       </c>
-      <c r="C145" t="n">
-        <v>0</v>
-      </c>
-      <c r="D145" t="n">
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
         <v>-0.36</v>
       </c>
-      <c r="E145" t="n">
+      <c r="E145">
         <v>-0.6</v>
       </c>
-      <c r="F145" t="n">
+      <c r="F145">
         <v>-0.38</v>
       </c>
-      <c r="G145" t="n">
+      <c r="G145">
         <v>0.61</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G145" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>